<commit_message>
feat: update test pattern gen
</commit_message>
<xml_diff>
--- a/FPGA/synth/math/multiplier/sim/test_data.xlsx
+++ b/FPGA/synth/math/multiplier/sim/test_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28110"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="526" documentId="11_3F8216BDF2DCCE836B02CE998F0AE45F5E522874" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73EC1677-F82A-42D3-A013-683E72B96094}"/>
+  <xr:revisionPtr revIDLastSave="655" documentId="11_3F8216BDF2DCCE836B02CE998F0AE45F5E522874" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BFF8E6C-3083-4781-9AAF-2C8BECBDBEBC}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -43,10 +43,27 @@
     <author>Motoki Kamimura</author>
   </authors>
   <commentList>
-    <comment ref="F2" authorId="0" shapeId="0" xr:uid="{ADDE4464-8DFC-45ED-AFE4-38EAD8AD5580}">
+    <comment ref="G4" authorId="0" shapeId="0" xr:uid="{ADDE4464-8DFC-45ED-AFE4-38EAD8AD5580}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="游ゴシック"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Motoki Kamimura:
+RANDBETWEEN() で生成した後、再現性確保のために固定した。</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G28" authorId="0" shapeId="0" xr:uid="{7913E922-01F6-4D70-9926-B43E91EB98AE}">
       <text>
         <t>Motoki Kamimura:
-RANDBETWEEN() で生成した後、再現性確保のために固定した。</t>
+乱数で生成した後に再現性確保のために固定した。
+元の数式は下記：
+=LET(A,POWER(2,$D$26-1),RANDBETWEEN(-A,A-1))</t>
       </text>
     </comment>
   </commentList>
@@ -76,7 +93,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="32">
+  <si>
+    <t>test_bench_fxd_pt_mul_sum_altera_vp_dsp_18x19_v1_0_0</t>
+  </si>
   <si>
     <t>parameter</t>
   </si>
@@ -139,6 +159,36 @@
   </si>
   <si>
     <t>EN_RND_HF2EVN</t>
+  </si>
+  <si>
+    <t>test_bench_cplx_mul_altera_vp_dsp_18x19</t>
+  </si>
+  <si>
+    <t>BW_IN_A</t>
+  </si>
+  <si>
+    <t>re_a</t>
+  </si>
+  <si>
+    <t>im_a</t>
+  </si>
+  <si>
+    <t>re_b</t>
+  </si>
+  <si>
+    <t>im_b</t>
+  </si>
+  <si>
+    <t>before slicing/rounding</t>
+  </si>
+  <si>
+    <t>re_c</t>
+  </si>
+  <si>
+    <t>im_c</t>
+  </si>
+  <si>
+    <t>BW_IN_B</t>
   </si>
 </sst>
 </file>
@@ -148,7 +198,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +212,12 @@
       <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="游ゴシック"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,19 +240,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -206,6 +256,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -561,886 +623,1907 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:O60"/>
+  <dimension ref="B2:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:J2"/>
+    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
-    <col min="1" max="1" width="3.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="3.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="9" width="10" style="1" customWidth="1"/>
-    <col min="10" max="10" width="6.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="1"/>
+    <col min="1" max="2" width="3.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="3.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="10" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="9" style="1"/>
+    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="45" customHeight="1">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:16">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+    </row>
+    <row r="4" spans="2:16" ht="45" customHeight="1">
+      <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="6" t="s">
+      <c r="G4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="5" t="s">
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="8" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="2:15" ht="39" customHeight="1">
-      <c r="B3" s="1" t="s">
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="5" spans="2:16" ht="39" customHeight="1">
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
         <v>18</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="2" t="s">
+      <c r="G5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="K5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O3" s="5"/>
-    </row>
-    <row r="4" spans="2:15" ht="15.75">
-      <c r="B4" s="1" t="s">
+      <c r="O5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="1">
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="2:16">
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1">
         <v>19</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F6" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="8">
+      <c r="G6" s="6">
         <v>33905</v>
       </c>
-      <c r="G4" s="8">
+      <c r="H6" s="6">
         <v>-122300</v>
       </c>
-      <c r="H4" s="8">
+      <c r="I6" s="6">
         <v>28174</v>
       </c>
-      <c r="I4" s="8">
+      <c r="J6" s="6">
         <v>123990</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K6" s="1">
         <v>1</v>
       </c>
-      <c r="K4" s="3">
-        <f>F4*G4+POWER(-1,J4)*H4*I4</f>
+      <c r="L6" s="2">
+        <f>G6*H6+POWER(-1,K6)*I6*J6</f>
         <v>-7639875760</v>
       </c>
-      <c r="L4" s="3" cm="1">
-        <f t="array" ref="L4">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K4))</f>
+      <c r="M6" s="2" cm="1">
+        <f t="array" ref="M6">ROUND_INT_HF2EVN($D$10,L6)</f>
         <v>-477492235</v>
       </c>
-      <c r="M4" s="3" cm="1">
-        <f t="array" ref="M4">UNSIGNED($C$3+$C$4+1-$C$8,L4)</f>
+      <c r="N6" s="2" cm="1">
+        <f t="array" ref="N6">UNSIGNED($D$5+$D$6+1-$D$10,M6)</f>
         <v>16702376949</v>
       </c>
-      <c r="N4" s="3" cm="1">
-        <f t="array" ref="N4">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M4)</f>
+      <c r="O6" s="2" cm="1">
+        <f t="array" ref="O6">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N6)</f>
         <v>3061</v>
       </c>
-      <c r="O4" s="3" cm="1">
-        <f t="array" ref="O4">SIGNED($C$7,N4)</f>
+      <c r="P6" s="2" cm="1">
+        <f t="array" ref="P6">SIGNED($D$9,O6)</f>
         <v>3061</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="15.75">
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1">
+    <row r="7" spans="2:16">
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
         <v>18</v>
       </c>
-      <c r="E5" s="1">
+      <c r="F7" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="8">
+      <c r="G7" s="6">
         <v>100428</v>
       </c>
-      <c r="G5" s="8">
+      <c r="H7" s="6">
         <v>192947</v>
       </c>
-      <c r="H5" s="8">
+      <c r="I7" s="6">
         <v>93946</v>
       </c>
-      <c r="I5" s="8">
+      <c r="J7" s="6">
         <v>-185078</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K7" s="1">
         <v>0</v>
       </c>
-      <c r="K5" s="3">
-        <f t="shared" ref="K5:K19" si="0">F5*G5+POWER(-1,J5)*H5*I5</f>
+      <c r="L7" s="2">
+        <f t="shared" ref="L7:L21" si="0">G7*H7+POWER(-1,K7)*I7*J7</f>
         <v>1989943528</v>
       </c>
-      <c r="L5" s="3" cm="1">
-        <f t="array" ref="L5">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K5))</f>
+      <c r="M7" s="2" cm="1">
+        <f t="array" ref="M7">ROUND_INT_HF2EVN($D$10,L7)</f>
         <v>124371470</v>
       </c>
-      <c r="M5" s="3" cm="1">
-        <f t="array" ref="M5">UNSIGNED($C$3+$C$4+1-$C$8,L5)</f>
+      <c r="N7" s="2" cm="1">
+        <f t="array" ref="N7">UNSIGNED($D$5+$D$6+1-$D$10,M7)</f>
         <v>124371470</v>
       </c>
-      <c r="N5" s="3" cm="1">
-        <f t="array" ref="N5">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M5)</f>
+      <c r="O7" s="2" cm="1">
+        <f t="array" ref="O7">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N7)</f>
         <v>49678</v>
       </c>
-      <c r="O5" s="3" cm="1">
-        <f t="array" ref="O5">SIGNED($C$7,N5)</f>
+      <c r="P7" s="2" cm="1">
+        <f t="array" ref="P7">SIGNED($D$9,O7)</f>
         <v>-15858</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="15.75">
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="1">
+    <row r="8" spans="2:16">
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1">
         <v>19</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="8">
+      <c r="G8" s="6">
         <v>-62914</v>
       </c>
-      <c r="G6" s="8">
+      <c r="H8" s="6">
         <v>207344</v>
       </c>
-      <c r="H6" s="8">
+      <c r="I8" s="6">
         <v>97977</v>
       </c>
-      <c r="I6" s="8">
+      <c r="J8" s="6">
         <v>-110722</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K8" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="3">
+      <c r="L8" s="2">
         <f t="shared" si="0"/>
         <v>-23893049810</v>
       </c>
-      <c r="L6" s="3" cm="1">
-        <f t="array" ref="L6">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K6))</f>
+      <c r="M8" s="2" cm="1">
+        <f t="array" ref="M8">ROUND_INT_HF2EVN($D$10,L8)</f>
         <v>-1493315613</v>
       </c>
-      <c r="M6" s="3" cm="1">
-        <f t="array" ref="M6">UNSIGNED($C$3+$C$4+1-$C$8,L6)</f>
+      <c r="N8" s="2" cm="1">
+        <f t="array" ref="N8">UNSIGNED($D$5+$D$6+1-$D$10,M8)</f>
         <v>15686553571</v>
       </c>
-      <c r="N6" s="3" cm="1">
-        <f t="array" ref="N6">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M6)</f>
+      <c r="O8" s="2" cm="1">
+        <f t="array" ref="O8">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N8)</f>
         <v>53219</v>
       </c>
-      <c r="O6" s="3" cm="1">
-        <f t="array" ref="O6">SIGNED($C$7,N6)</f>
+      <c r="P8" s="2" cm="1">
+        <f t="array" ref="P8">SIGNED($D$9,O8)</f>
         <v>-12317</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="15.75">
-      <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="1">
+    <row r="9" spans="2:16">
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1">
         <v>16</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F9" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="8">
+      <c r="G9" s="6">
         <v>54938</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H9" s="6">
         <v>-40849</v>
       </c>
-      <c r="H7" s="8">
+      <c r="I9" s="6">
         <v>-86956</v>
       </c>
-      <c r="I7" s="8">
+      <c r="J9" s="6">
         <v>261622</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K9" s="1">
         <v>0</v>
       </c>
-      <c r="K7" s="3">
+      <c r="L9" s="2">
         <f t="shared" si="0"/>
         <v>-24993764994</v>
       </c>
-      <c r="L7" s="3" cm="1">
-        <f t="array" ref="L7">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K7))</f>
+      <c r="M9" s="2" cm="1">
+        <f t="array" ref="M9">ROUND_INT_HF2EVN($D$10,L9)</f>
         <v>-1562110312</v>
       </c>
-      <c r="M7" s="3" cm="1">
-        <f t="array" ref="M7">UNSIGNED($C$3+$C$4+1-$C$8,L7)</f>
+      <c r="N9" s="2" cm="1">
+        <f t="array" ref="N9">UNSIGNED($D$5+$D$6+1-$D$10,M9)</f>
         <v>15617758872</v>
       </c>
-      <c r="N7" s="3" cm="1">
-        <f t="array" ref="N7">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M7)</f>
+      <c r="O9" s="2" cm="1">
+        <f t="array" ref="O9">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N9)</f>
         <v>5784</v>
       </c>
-      <c r="O7" s="3" cm="1">
-        <f t="array" ref="O7">SIGNED($C$7,N7)</f>
+      <c r="P9" s="2" cm="1">
+        <f t="array" ref="P9">SIGNED($D$9,O9)</f>
         <v>5784</v>
       </c>
     </row>
-    <row r="8" spans="2:15" ht="15.75">
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1">
+    <row r="10" spans="2:16">
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="1">
         <v>4</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F10" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="8">
+      <c r="G10" s="6">
         <v>-72284</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H10" s="6">
         <v>-261782</v>
       </c>
-      <c r="H8" s="8">
+      <c r="I10" s="6">
         <v>129660</v>
       </c>
-      <c r="I8" s="8">
+      <c r="J10" s="6">
         <v>150541</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K10" s="1">
         <v>0</v>
       </c>
-      <c r="K8" s="3">
+      <c r="L10" s="2">
         <f t="shared" si="0"/>
         <v>38441796148</v>
       </c>
-      <c r="L8" s="3" cm="1">
-        <f t="array" ref="L8">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K8))</f>
+      <c r="M10" s="2" cm="1">
+        <f t="array" ref="M10">ROUND_INT_HF2EVN($D$10,L10)</f>
         <v>2402612259</v>
       </c>
-      <c r="M8" s="3" cm="1">
-        <f t="array" ref="M8">UNSIGNED($C$3+$C$4+1-$C$8,L8)</f>
+      <c r="N10" s="2" cm="1">
+        <f t="array" ref="N10">UNSIGNED($D$5+$D$6+1-$D$10,M10)</f>
         <v>2402612259</v>
       </c>
-      <c r="N8" s="3" cm="1">
-        <f t="array" ref="N8">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M8)</f>
+      <c r="O10" s="2" cm="1">
+        <f t="array" ref="O10">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N10)</f>
         <v>62499</v>
       </c>
-      <c r="O8" s="3" cm="1">
-        <f t="array" ref="O8">SIGNED($C$7,N8)</f>
+      <c r="P10" s="2" cm="1">
+        <f t="array" ref="P10">SIGNED($D$9,O10)</f>
         <v>-3037</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15.75">
-      <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1">
+    <row r="11" spans="2:16">
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F11" s="1">
         <v>5</v>
       </c>
-      <c r="F9" s="8">
+      <c r="G11" s="6">
         <v>-103773</v>
       </c>
-      <c r="G9" s="8">
+      <c r="H11" s="6">
         <v>12691</v>
       </c>
-      <c r="H9" s="8">
+      <c r="I11" s="6">
         <v>-39509</v>
       </c>
-      <c r="I9" s="8">
+      <c r="J11" s="6">
         <v>-115333</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K11" s="1">
         <v>0</v>
       </c>
-      <c r="K9" s="3">
+      <c r="L11" s="2">
         <f t="shared" si="0"/>
         <v>3239708354</v>
       </c>
-      <c r="L9" s="3" cm="1">
-        <f t="array" ref="L9">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K9))</f>
+      <c r="M11" s="2" cm="1">
+        <f t="array" ref="M11">ROUND_INT_HF2EVN($D$10,L11)</f>
         <v>202481772</v>
       </c>
-      <c r="M9" s="3" cm="1">
-        <f t="array" ref="M9">UNSIGNED($C$3+$C$4+1-$C$8,L9)</f>
+      <c r="N11" s="2" cm="1">
+        <f t="array" ref="N11">UNSIGNED($D$5+$D$6+1-$D$10,M11)</f>
         <v>202481772</v>
       </c>
-      <c r="N9" s="3" cm="1">
-        <f t="array" ref="N9">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M9)</f>
+      <c r="O11" s="2" cm="1">
+        <f t="array" ref="O11">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N11)</f>
         <v>41068</v>
       </c>
-      <c r="O9" s="3" cm="1">
-        <f t="array" ref="O9">SIGNED($C$7,N9)</f>
+      <c r="P11" s="2" cm="1">
+        <f t="array" ref="P11">SIGNED($D$9,O11)</f>
         <v>-24468</v>
       </c>
     </row>
-    <row r="10" spans="2:15" ht="15.75">
-      <c r="E10" s="1">
+    <row r="12" spans="2:16">
+      <c r="F12" s="1">
         <v>6</v>
       </c>
-      <c r="F10" s="8">
+      <c r="G12" s="6">
         <v>84523</v>
       </c>
-      <c r="G10" s="8">
+      <c r="H12" s="6">
         <v>-168039</v>
       </c>
-      <c r="H10" s="8">
+      <c r="I12" s="6">
         <v>122818</v>
       </c>
-      <c r="I10" s="8">
+      <c r="J12" s="6">
         <v>-202889</v>
       </c>
-      <c r="J10" s="1">
+      <c r="K12" s="1">
         <v>0</v>
       </c>
-      <c r="K10" s="3">
+      <c r="L12" s="2">
         <f t="shared" si="0"/>
         <v>-39121581599</v>
       </c>
-      <c r="L10" s="3" cm="1">
-        <f t="array" ref="L10">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K10))</f>
+      <c r="M12" s="2" cm="1">
+        <f t="array" ref="M12">ROUND_INT_HF2EVN($D$10,L12)</f>
         <v>-2445098850</v>
       </c>
-      <c r="M10" s="3" cm="1">
-        <f t="array" ref="M10">UNSIGNED($C$3+$C$4+1-$C$8,L10)</f>
+      <c r="N12" s="2" cm="1">
+        <f t="array" ref="N12">UNSIGNED($D$5+$D$6+1-$D$10,M12)</f>
         <v>14734770334</v>
       </c>
-      <c r="N10" s="3" cm="1">
-        <f t="array" ref="N10">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M10)</f>
+      <c r="O12" s="2" cm="1">
+        <f t="array" ref="O12">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N12)</f>
         <v>49310</v>
       </c>
-      <c r="O10" s="3" cm="1">
-        <f t="array" ref="O10">SIGNED($C$7,N10)</f>
+      <c r="P12" s="2" cm="1">
+        <f t="array" ref="P12">SIGNED($D$9,O12)</f>
         <v>-16226</v>
       </c>
     </row>
-    <row r="11" spans="2:15" ht="15.75">
-      <c r="E11" s="1">
+    <row r="13" spans="2:16">
+      <c r="F13" s="1">
         <v>7</v>
       </c>
-      <c r="F11" s="8">
+      <c r="G13" s="6">
         <v>49972</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H13" s="6">
         <v>-190779</v>
       </c>
-      <c r="H11" s="8">
+      <c r="I13" s="6">
         <v>64731</v>
       </c>
-      <c r="I11" s="8">
+      <c r="J13" s="6">
         <v>-128147</v>
       </c>
-      <c r="J11" s="1">
+      <c r="K13" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="3">
+      <c r="L13" s="2">
         <f t="shared" si="0"/>
         <v>-17828691645</v>
       </c>
-      <c r="L11" s="3" cm="1">
-        <f t="array" ref="L11">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K11))</f>
+      <c r="M13" s="2" cm="1">
+        <f t="array" ref="M13">ROUND_INT_HF2EVN($D$10,L13)</f>
         <v>-1114293228</v>
       </c>
-      <c r="M11" s="3" cm="1">
-        <f t="array" ref="M11">UNSIGNED($C$3+$C$4+1-$C$8,L11)</f>
+      <c r="N13" s="2" cm="1">
+        <f t="array" ref="N13">UNSIGNED($D$5+$D$6+1-$D$10,M13)</f>
         <v>16065575956</v>
       </c>
-      <c r="N11" s="3" cm="1">
-        <f t="array" ref="N11">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M11)</f>
+      <c r="O13" s="2" cm="1">
+        <f t="array" ref="O13">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N13)</f>
         <v>15380</v>
       </c>
-      <c r="O11" s="3" cm="1">
-        <f t="array" ref="O11">SIGNED($C$7,N11)</f>
+      <c r="P13" s="2" cm="1">
+        <f t="array" ref="P13">SIGNED($D$9,O13)</f>
         <v>15380</v>
       </c>
     </row>
-    <row r="12" spans="2:15" ht="15.75">
-      <c r="E12" s="1">
+    <row r="14" spans="2:16">
+      <c r="F14" s="1">
         <v>8</v>
       </c>
-      <c r="F12" s="8">
+      <c r="G14" s="6">
         <v>9678</v>
       </c>
-      <c r="G12" s="8">
+      <c r="H14" s="6">
         <v>13815</v>
       </c>
-      <c r="H12" s="8">
+      <c r="I14" s="6">
         <v>18102</v>
       </c>
-      <c r="I12" s="8">
+      <c r="J14" s="6">
         <v>-182979</v>
       </c>
-      <c r="J12" s="1">
+      <c r="K14" s="1">
         <v>0</v>
       </c>
-      <c r="K12" s="3">
+      <c r="L14" s="2">
         <f t="shared" si="0"/>
         <v>-3178584288</v>
       </c>
-      <c r="L12" s="3" cm="1">
-        <f t="array" ref="L12">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K12))</f>
+      <c r="M14" s="2" cm="1">
+        <f t="array" ref="M14">ROUND_INT_HF2EVN($D$10,L14)</f>
         <v>-198661518</v>
       </c>
-      <c r="M12" s="3" cm="1">
-        <f t="array" ref="M12">UNSIGNED($C$3+$C$4+1-$C$8,L12)</f>
+      <c r="N14" s="2" cm="1">
+        <f t="array" ref="N14">UNSIGNED($D$5+$D$6+1-$D$10,M14)</f>
         <v>16981207666</v>
       </c>
-      <c r="N12" s="3" cm="1">
-        <f t="array" ref="N12">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M12)</f>
+      <c r="O14" s="2" cm="1">
+        <f t="array" ref="O14">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N14)</f>
         <v>43634</v>
       </c>
-      <c r="O12" s="3" cm="1">
-        <f t="array" ref="O12">SIGNED($C$7,N12)</f>
+      <c r="P14" s="2" cm="1">
+        <f t="array" ref="P14">SIGNED($D$9,O14)</f>
         <v>-21902</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="15.75">
-      <c r="E13" s="1">
+    <row r="15" spans="2:16">
+      <c r="F15" s="1">
         <v>9</v>
       </c>
-      <c r="F13" s="8">
+      <c r="G15" s="6">
         <v>-19611</v>
       </c>
-      <c r="G13" s="8">
+      <c r="H15" s="6">
         <v>-244298</v>
       </c>
-      <c r="H13" s="8">
+      <c r="I15" s="6">
         <v>82165</v>
       </c>
-      <c r="I13" s="8">
+      <c r="J15" s="6">
         <v>-34428</v>
       </c>
-      <c r="J13" s="1">
+      <c r="K15" s="1">
         <v>1</v>
       </c>
-      <c r="K13" s="3">
+      <c r="L15" s="2">
         <f t="shared" si="0"/>
         <v>7619704698</v>
       </c>
-      <c r="L13" s="3" cm="1">
-        <f t="array" ref="L13">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K13))</f>
+      <c r="M15" s="2" cm="1">
+        <f t="array" ref="M15">ROUND_INT_HF2EVN($D$10,L15)</f>
         <v>476231544</v>
       </c>
-      <c r="M13" s="3" cm="1">
-        <f t="array" ref="M13">UNSIGNED($C$3+$C$4+1-$C$8,L13)</f>
+      <c r="N15" s="2" cm="1">
+        <f t="array" ref="N15">UNSIGNED($D$5+$D$6+1-$D$10,M15)</f>
         <v>476231544</v>
       </c>
-      <c r="N13" s="3" cm="1">
-        <f t="array" ref="N13">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M13)</f>
+      <c r="O15" s="2" cm="1">
+        <f t="array" ref="O15">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N15)</f>
         <v>46968</v>
       </c>
-      <c r="O13" s="3" cm="1">
-        <f t="array" ref="O13">SIGNED($C$7,N13)</f>
+      <c r="P15" s="2" cm="1">
+        <f t="array" ref="P15">SIGNED($D$9,O15)</f>
         <v>-18568</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="15.75">
-      <c r="E14" s="1">
+    <row r="16" spans="2:16">
+      <c r="F16" s="1">
         <v>10</v>
       </c>
-      <c r="F14" s="8">
+      <c r="G16" s="6">
         <v>67102</v>
       </c>
-      <c r="G14" s="8">
+      <c r="H16" s="6">
         <v>-18595</v>
       </c>
-      <c r="H14" s="8">
+      <c r="I16" s="6">
         <v>102809</v>
       </c>
-      <c r="I14" s="8">
+      <c r="J16" s="6">
         <v>44813</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K16" s="1">
         <v>1</v>
       </c>
-      <c r="K14" s="3">
+      <c r="L16" s="2">
         <f t="shared" si="0"/>
         <v>-5854941407</v>
       </c>
-      <c r="L14" s="3" cm="1">
-        <f t="array" ref="L14">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K14))</f>
+      <c r="M16" s="2" cm="1">
+        <f t="array" ref="M16">ROUND_INT_HF2EVN($D$10,L16)</f>
         <v>-365933838</v>
       </c>
-      <c r="M14" s="3" cm="1">
-        <f t="array" ref="M14">UNSIGNED($C$3+$C$4+1-$C$8,L14)</f>
+      <c r="N16" s="2" cm="1">
+        <f t="array" ref="N16">UNSIGNED($D$5+$D$6+1-$D$10,M16)</f>
         <v>16813935346</v>
       </c>
-      <c r="N14" s="3" cm="1">
-        <f t="array" ref="N14">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M14)</f>
+      <c r="O16" s="2" cm="1">
+        <f t="array" ref="O16">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N16)</f>
         <v>19186</v>
       </c>
-      <c r="O14" s="3" cm="1">
-        <f t="array" ref="O14">SIGNED($C$7,N14)</f>
+      <c r="P16" s="2" cm="1">
+        <f t="array" ref="P16">SIGNED($D$9,O16)</f>
         <v>19186</v>
       </c>
     </row>
-    <row r="15" spans="2:15" ht="15.75">
-      <c r="E15" s="1">
+    <row r="17" spans="2:20">
+      <c r="F17" s="1">
         <v>11</v>
       </c>
-      <c r="F15" s="8">
+      <c r="G17" s="6">
         <v>94175</v>
       </c>
-      <c r="G15" s="8">
+      <c r="H17" s="6">
         <v>9863</v>
       </c>
-      <c r="H15" s="8">
+      <c r="I17" s="6">
         <v>45353</v>
       </c>
-      <c r="I15" s="8">
+      <c r="J17" s="6">
         <v>33580</v>
       </c>
-      <c r="J15" s="1">
+      <c r="K17" s="1">
         <v>0</v>
       </c>
-      <c r="K15" s="3">
+      <c r="L17" s="2">
         <f t="shared" si="0"/>
         <v>2451801765</v>
       </c>
-      <c r="L15" s="3" cm="1">
-        <f t="array" ref="L15">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K15))</f>
+      <c r="M17" s="2" cm="1">
+        <f t="array" ref="M17">ROUND_INT_HF2EVN($D$10,L17)</f>
         <v>153237610</v>
       </c>
-      <c r="M15" s="3" cm="1">
-        <f t="array" ref="M15">UNSIGNED($C$3+$C$4+1-$C$8,L15)</f>
+      <c r="N17" s="2" cm="1">
+        <f t="array" ref="N17">UNSIGNED($D$5+$D$6+1-$D$10,M17)</f>
         <v>153237610</v>
       </c>
-      <c r="N15" s="3" cm="1">
-        <f t="array" ref="N15">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M15)</f>
+      <c r="O17" s="2" cm="1">
+        <f t="array" ref="O17">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N17)</f>
         <v>14442</v>
       </c>
-      <c r="O15" s="3" cm="1">
-        <f t="array" ref="O15">SIGNED($C$7,N15)</f>
+      <c r="P17" s="2" cm="1">
+        <f t="array" ref="P17">SIGNED($D$9,O17)</f>
         <v>14442</v>
       </c>
     </row>
-    <row r="16" spans="2:15" ht="15.75">
-      <c r="E16" s="1">
+    <row r="18" spans="2:20">
+      <c r="F18" s="1">
         <v>12</v>
       </c>
-      <c r="F16" s="8">
+      <c r="G18" s="6">
         <v>25821</v>
       </c>
-      <c r="G16" s="8">
+      <c r="H18" s="6">
         <v>248060</v>
       </c>
-      <c r="H16" s="7">
+      <c r="I18" s="5">
         <v>-679</v>
       </c>
-      <c r="I16" s="8">
+      <c r="J18" s="6">
         <v>97914</v>
       </c>
-      <c r="J16" s="1">
+      <c r="K18" s="1">
         <v>0</v>
       </c>
-      <c r="K16" s="3">
+      <c r="L18" s="2">
         <f t="shared" si="0"/>
         <v>6338673654</v>
       </c>
-      <c r="L16" s="3" cm="1">
-        <f t="array" ref="L16">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K16))</f>
+      <c r="M18" s="2" cm="1">
+        <f t="array" ref="M18">ROUND_INT_HF2EVN($D$10,L18)</f>
         <v>396167103</v>
       </c>
-      <c r="M16" s="3" cm="1">
-        <f t="array" ref="M16">UNSIGNED($C$3+$C$4+1-$C$8,L16)</f>
+      <c r="N18" s="2" cm="1">
+        <f t="array" ref="N18">UNSIGNED($D$5+$D$6+1-$D$10,M18)</f>
         <v>396167103</v>
       </c>
-      <c r="N16" s="3" cm="1">
-        <f t="array" ref="N16">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M16)</f>
+      <c r="O18" s="2" cm="1">
+        <f t="array" ref="O18">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N18)</f>
         <v>1983</v>
       </c>
-      <c r="O16" s="3" cm="1">
-        <f t="array" ref="O16">SIGNED($C$7,N16)</f>
+      <c r="P18" s="2" cm="1">
+        <f t="array" ref="P18">SIGNED($D$9,O18)</f>
         <v>1983</v>
       </c>
     </row>
-    <row r="17" spans="5:15" ht="15.75">
-      <c r="E17" s="1">
+    <row r="19" spans="2:20">
+      <c r="F19" s="1">
         <v>13</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G19" s="6">
         <v>41716</v>
       </c>
-      <c r="G17" s="8">
+      <c r="H19" s="6">
         <v>-19937</v>
       </c>
-      <c r="H17" s="8">
+      <c r="I19" s="6">
         <v>95565</v>
       </c>
-      <c r="I17" s="8">
+      <c r="J19" s="6">
         <v>167240</v>
       </c>
-      <c r="J17" s="1">
+      <c r="K19" s="1">
         <v>0</v>
       </c>
-      <c r="K17" s="3">
+      <c r="L19" s="2">
         <f t="shared" si="0"/>
         <v>15150598708</v>
       </c>
-      <c r="L17" s="3" cm="1">
-        <f t="array" ref="L17">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K17))</f>
+      <c r="M19" s="2" cm="1">
+        <f t="array" ref="M19">ROUND_INT_HF2EVN($D$10,L19)</f>
         <v>946912419</v>
       </c>
-      <c r="M17" s="3" cm="1">
-        <f t="array" ref="M17">UNSIGNED($C$3+$C$4+1-$C$8,L17)</f>
+      <c r="N19" s="2" cm="1">
+        <f t="array" ref="N19">UNSIGNED($D$5+$D$6+1-$D$10,M19)</f>
         <v>946912419</v>
       </c>
-      <c r="N17" s="3" cm="1">
-        <f t="array" ref="N17">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M17)</f>
+      <c r="O19" s="2" cm="1">
+        <f t="array" ref="O19">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N19)</f>
         <v>48291</v>
       </c>
-      <c r="O17" s="3" cm="1">
-        <f t="array" ref="O17">SIGNED($C$7,N17)</f>
+      <c r="P19" s="2" cm="1">
+        <f t="array" ref="P19">SIGNED($D$9,O19)</f>
         <v>-17245</v>
       </c>
     </row>
-    <row r="18" spans="5:15" ht="15.75">
-      <c r="E18" s="1">
+    <row r="20" spans="2:20">
+      <c r="F20" s="1">
         <v>14</v>
       </c>
-      <c r="F18" s="8">
+      <c r="G20" s="6">
         <v>-2225</v>
       </c>
-      <c r="G18" s="8">
+      <c r="H20" s="6">
         <v>-232473</v>
       </c>
-      <c r="H18" s="8">
+      <c r="I20" s="6">
         <v>120462</v>
       </c>
-      <c r="I18" s="8">
+      <c r="J20" s="6">
         <v>-92275</v>
       </c>
-      <c r="J18" s="1">
+      <c r="K20" s="1">
         <v>0</v>
       </c>
-      <c r="K18" s="3">
+      <c r="L20" s="2">
         <f t="shared" si="0"/>
         <v>-10598378625</v>
       </c>
-      <c r="L18" s="3" cm="1">
-        <f t="array" ref="L18">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K18))</f>
+      <c r="M20" s="2" cm="1">
+        <f t="array" ref="M20">ROUND_INT_HF2EVN($D$10,L20)</f>
         <v>-662398664</v>
       </c>
-      <c r="M18" s="3" cm="1">
-        <f t="array" ref="M18">UNSIGNED($C$3+$C$4+1-$C$8,L18)</f>
+      <c r="N20" s="2" cm="1">
+        <f t="array" ref="N20">UNSIGNED($D$5+$D$6+1-$D$10,M20)</f>
         <v>16517470520</v>
       </c>
-      <c r="N18" s="3" cm="1">
-        <f t="array" ref="N18">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M18)</f>
+      <c r="O20" s="2" cm="1">
+        <f t="array" ref="O20">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N20)</f>
         <v>39224</v>
       </c>
-      <c r="O18" s="3" cm="1">
-        <f t="array" ref="O18">SIGNED($C$7,N18)</f>
+      <c r="P20" s="2" cm="1">
+        <f t="array" ref="P20">SIGNED($D$9,O20)</f>
         <v>-26312</v>
       </c>
     </row>
-    <row r="19" spans="5:15" ht="15.75">
-      <c r="E19" s="1">
+    <row r="21" spans="2:20">
+      <c r="F21" s="1">
         <v>15</v>
       </c>
-      <c r="F19" s="8">
+      <c r="G21" s="6">
         <v>-11091</v>
       </c>
-      <c r="G19" s="8">
+      <c r="H21" s="6">
         <v>-162575</v>
       </c>
-      <c r="H19" s="8">
+      <c r="I21" s="6">
         <v>-101848</v>
       </c>
-      <c r="I19" s="8">
+      <c r="J21" s="6">
         <v>-155845</v>
       </c>
-      <c r="J19" s="1">
+      <c r="K21" s="1">
         <v>0</v>
       </c>
-      <c r="K19" s="3">
+      <c r="L21" s="2">
         <f t="shared" si="0"/>
         <v>17675620885</v>
       </c>
-      <c r="L19" s="3" cm="1">
-        <f t="array" ref="L19">IF($C$9=0,"N/A",ROUND_INT_HF2EVN($C$8,K19))</f>
+      <c r="M21" s="2" cm="1">
+        <f t="array" ref="M21">ROUND_INT_HF2EVN($D$10,L21)</f>
         <v>1104726305</v>
       </c>
-      <c r="M19" s="3" cm="1">
-        <f t="array" ref="M19">UNSIGNED($C$3+$C$4+1-$C$8,L19)</f>
+      <c r="N21" s="2" cm="1">
+        <f t="array" ref="N21">UNSIGNED($D$5+$D$6+1-$D$10,M21)</f>
         <v>1104726305</v>
       </c>
-      <c r="N19" s="3" cm="1">
-        <f t="array" ref="N19">BIT_SLICE($C$3+$C$4+1-$C$8,0,$C$7,M19)</f>
+      <c r="O21" s="2" cm="1">
+        <f t="array" ref="O21">BIT_SLICE($D$5+$D$6+1-$D$10,0,$D$9,N21)</f>
         <v>51489</v>
       </c>
-      <c r="O19" s="3" cm="1">
-        <f t="array" ref="O19">SIGNED($C$7,N19)</f>
+      <c r="P21" s="2" cm="1">
+        <f t="array" ref="P21">SIGNED($D$9,O21)</f>
         <v>-14047</v>
       </c>
     </row>
-    <row r="20" spans="5:15">
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="5:15">
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="5:15">
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="5:15">
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="5:15">
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="5:15">
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="5:15">
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="5:15">
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="5:15">
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="5:15">
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="5:15">
-      <c r="G30" s="2"/>
-    </row>
-    <row r="31" spans="5:15">
-      <c r="G31" s="2"/>
-    </row>
-    <row r="32" spans="5:15">
-      <c r="G32" s="2"/>
-    </row>
-    <row r="35" spans="3:7">
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-    </row>
-    <row r="36" spans="3:7">
-      <c r="C36" s="2"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="5"/>
-    </row>
-    <row r="47" spans="3:7">
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-    </row>
-    <row r="48" spans="3:7">
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-    </row>
-    <row r="49" spans="3:8">
-      <c r="G49" s="2"/>
-    </row>
-    <row r="50" spans="3:8">
-      <c r="G50" s="2"/>
-    </row>
-    <row r="51" spans="3:8">
-      <c r="G51" s="2"/>
-    </row>
-    <row r="52" spans="3:8">
-      <c r="G52" s="2"/>
-    </row>
-    <row r="53" spans="3:8">
-      <c r="G53" s="2"/>
-    </row>
-    <row r="54" spans="3:8">
-      <c r="G54" s="2"/>
-    </row>
-    <row r="55" spans="3:8">
-      <c r="G55" s="2"/>
-    </row>
-    <row r="56" spans="3:8">
-      <c r="G56" s="2"/>
-    </row>
-    <row r="59" spans="3:8">
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-    </row>
-    <row r="60" spans="3:8">
-      <c r="C60" s="2"/>
-      <c r="D60" s="2"/>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2"/>
-      <c r="G60" s="2"/>
-      <c r="H60" s="5"/>
+    <row r="22" spans="2:20">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:20">
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="2:20">
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="2:20">
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
+      <c r="N25" s="10"/>
+      <c r="O25" s="10"/>
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10"/>
+      <c r="R25" s="10"/>
+      <c r="S25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="T25" s="7"/>
+    </row>
+    <row r="26" spans="2:20">
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="1">
+        <v>18</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J26" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="2:20">
+      <c r="C27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="1">
+        <v>19</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q27" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="R27" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+    </row>
+    <row r="28" spans="2:20">
+      <c r="C28" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="1">
+        <v>16</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="9">
+        <v>-28538</v>
+      </c>
+      <c r="H28" s="9">
+        <v>-127202</v>
+      </c>
+      <c r="I28" s="9">
+        <v>-184004</v>
+      </c>
+      <c r="J28" s="9">
+        <v>13277</v>
+      </c>
+      <c r="K28" s="2">
+        <f>$G28*$I28-$H28*$J28</f>
+        <v>6939967106</v>
+      </c>
+      <c r="L28" s="2">
+        <f>G28*J28+H28*I28</f>
+        <v>23026777782</v>
+      </c>
+      <c r="M28" s="2" cm="1">
+        <f t="array" ref="M28">ROUND_INT_HF2EVN($D$29,K28)</f>
+        <v>433747944</v>
+      </c>
+      <c r="N28" s="2" cm="1">
+        <f t="array" ref="N28">ROUND_INT_HF2EVN($D$29,L28)</f>
+        <v>1439173611</v>
+      </c>
+      <c r="O28" s="2" cm="1">
+        <f t="array" ref="O28">UNSIGNED($D$26+$D$27+1-$D$29,M28)</f>
+        <v>433747944</v>
+      </c>
+      <c r="P28" s="2" cm="1">
+        <f t="array" ref="P28">UNSIGNED($D$26+$D$27+1-$D$29,N28)</f>
+        <v>1439173611</v>
+      </c>
+      <c r="Q28" s="2" cm="1">
+        <f t="array" ref="Q28">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O28)</f>
+        <v>30696</v>
+      </c>
+      <c r="R28" s="2" cm="1">
+        <f t="array" ref="R28">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P28)</f>
+        <v>3051</v>
+      </c>
+      <c r="S28" s="2" cm="1">
+        <f t="array" ref="S28">SIGNED($D$28,Q28)</f>
+        <v>30696</v>
+      </c>
+      <c r="T28" s="2" cm="1">
+        <f t="array" ref="T28">SIGNED($D$28,R28)</f>
+        <v>3051</v>
+      </c>
+    </row>
+    <row r="29" spans="2:20">
+      <c r="C29" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="1">
+        <v>4</v>
+      </c>
+      <c r="F29" s="1">
+        <v>1</v>
+      </c>
+      <c r="G29" s="9">
+        <v>106182</v>
+      </c>
+      <c r="H29" s="9">
+        <v>-117151</v>
+      </c>
+      <c r="I29" s="9">
+        <v>138179</v>
+      </c>
+      <c r="J29" s="9">
+        <v>242635</v>
+      </c>
+      <c r="K29" s="2">
+        <f t="shared" ref="K29:K43" si="1">$G29*$I29-$H29*$J29</f>
+        <v>43097055463</v>
+      </c>
+      <c r="L29" s="2">
+        <f t="shared" ref="L29:L43" si="2">G29*J29+H29*I29</f>
+        <v>9575661541</v>
+      </c>
+      <c r="M29" s="2" cm="1">
+        <f t="array" ref="M29">ROUND_INT_HF2EVN($D$29,K29)</f>
+        <v>2693565966</v>
+      </c>
+      <c r="N29" s="2" cm="1">
+        <f t="array" ref="N29">ROUND_INT_HF2EVN($D$29,L29)</f>
+        <v>598478846</v>
+      </c>
+      <c r="O29" s="2" cm="1">
+        <f t="array" ref="O29">UNSIGNED($D$26+$D$27+1-$D$29,M29)</f>
+        <v>2693565966</v>
+      </c>
+      <c r="P29" s="2" cm="1">
+        <f t="array" ref="P29">UNSIGNED($D$26+$D$27+1-$D$29,N29)</f>
+        <v>598478846</v>
+      </c>
+      <c r="Q29" s="2" cm="1">
+        <f t="array" ref="Q29">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O29)</f>
+        <v>36366</v>
+      </c>
+      <c r="R29" s="2" cm="1">
+        <f t="array" ref="R29">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P29)</f>
+        <v>4094</v>
+      </c>
+      <c r="S29" s="2" cm="1">
+        <f t="array" ref="S29">SIGNED($D$28,Q29)</f>
+        <v>-29170</v>
+      </c>
+      <c r="T29" s="2" cm="1">
+        <f t="array" ref="T29">SIGNED($D$28,R29)</f>
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="30" spans="2:20">
+      <c r="C30" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9">
+        <v>-7117</v>
+      </c>
+      <c r="H30" s="9">
+        <v>80541</v>
+      </c>
+      <c r="I30" s="9">
+        <v>175606</v>
+      </c>
+      <c r="J30" s="9">
+        <v>147324</v>
+      </c>
+      <c r="K30" s="2">
+        <f t="shared" si="1"/>
+        <v>-13115410186</v>
+      </c>
+      <c r="L30" s="2">
+        <f t="shared" si="2"/>
+        <v>13094977938</v>
+      </c>
+      <c r="M30" s="2" cm="1">
+        <f t="array" ref="M30">ROUND_INT_HF2EVN($D$29,K30)</f>
+        <v>-819713137</v>
+      </c>
+      <c r="N30" s="2" cm="1">
+        <f t="array" ref="N30">ROUND_INT_HF2EVN($D$29,L30)</f>
+        <v>818436121</v>
+      </c>
+      <c r="O30" s="2" cm="1">
+        <f t="array" ref="O30">UNSIGNED($D$26+$D$27+1-$D$29,M30)</f>
+        <v>16360156047</v>
+      </c>
+      <c r="P30" s="2" cm="1">
+        <f t="array" ref="P30">UNSIGNED($D$26+$D$27+1-$D$29,N30)</f>
+        <v>818436121</v>
+      </c>
+      <c r="Q30" s="2" cm="1">
+        <f t="array" ref="Q30">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O30)</f>
+        <v>11151</v>
+      </c>
+      <c r="R30" s="2" cm="1">
+        <f t="array" ref="R30">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P30)</f>
+        <v>22553</v>
+      </c>
+      <c r="S30" s="2" cm="1">
+        <f t="array" ref="S30">SIGNED($D$28,Q30)</f>
+        <v>11151</v>
+      </c>
+      <c r="T30" s="2" cm="1">
+        <f t="array" ref="T30">SIGNED($D$28,R30)</f>
+        <v>22553</v>
+      </c>
+    </row>
+    <row r="31" spans="2:20">
+      <c r="F31" s="1">
+        <v>3</v>
+      </c>
+      <c r="G31" s="9">
+        <v>-119900</v>
+      </c>
+      <c r="H31" s="9">
+        <v>-18819</v>
+      </c>
+      <c r="I31" s="9">
+        <v>-16301</v>
+      </c>
+      <c r="J31" s="9">
+        <v>107207</v>
+      </c>
+      <c r="K31" s="2">
+        <f t="shared" si="1"/>
+        <v>3972018433</v>
+      </c>
+      <c r="L31" s="2">
+        <f t="shared" si="2"/>
+        <v>-12547350781</v>
+      </c>
+      <c r="M31" s="2" cm="1">
+        <f t="array" ref="M31">ROUND_INT_HF2EVN($D$29,K31)</f>
+        <v>248251152</v>
+      </c>
+      <c r="N31" s="2" cm="1">
+        <f t="array" ref="N31">ROUND_INT_HF2EVN($D$29,L31)</f>
+        <v>-784209424</v>
+      </c>
+      <c r="O31" s="2" cm="1">
+        <f t="array" ref="O31">UNSIGNED($D$26+$D$27+1-$D$29,M31)</f>
+        <v>248251152</v>
+      </c>
+      <c r="P31" s="2" cm="1">
+        <f t="array" ref="P31">UNSIGNED($D$26+$D$27+1-$D$29,N31)</f>
+        <v>16395659760</v>
+      </c>
+      <c r="Q31" s="2" cm="1">
+        <f t="array" ref="Q31">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O31)</f>
+        <v>784</v>
+      </c>
+      <c r="R31" s="2" cm="1">
+        <f t="array" ref="R31">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P31)</f>
+        <v>59888</v>
+      </c>
+      <c r="S31" s="2" cm="1">
+        <f t="array" ref="S31">SIGNED($D$28,Q31)</f>
+        <v>784</v>
+      </c>
+      <c r="T31" s="2" cm="1">
+        <f t="array" ref="T31">SIGNED($D$28,R31)</f>
+        <v>-5648</v>
+      </c>
+    </row>
+    <row r="32" spans="2:20">
+      <c r="F32" s="1">
+        <v>4</v>
+      </c>
+      <c r="G32" s="9">
+        <v>107635</v>
+      </c>
+      <c r="H32" s="9">
+        <v>-54437</v>
+      </c>
+      <c r="I32" s="9">
+        <v>-231955</v>
+      </c>
+      <c r="J32" s="9">
+        <v>-24275</v>
+      </c>
+      <c r="K32" s="2">
+        <f t="shared" si="1"/>
+        <v>-26287934600</v>
+      </c>
+      <c r="L32" s="2">
+        <f t="shared" si="2"/>
+        <v>10014094710</v>
+      </c>
+      <c r="M32" s="2" cm="1">
+        <f t="array" ref="M32">ROUND_INT_HF2EVN($D$29,K32)</f>
+        <v>-1642995912</v>
+      </c>
+      <c r="N32" s="2" cm="1">
+        <f t="array" ref="N32">ROUND_INT_HF2EVN($D$29,L32)</f>
+        <v>625880919</v>
+      </c>
+      <c r="O32" s="2" cm="1">
+        <f t="array" ref="O32">UNSIGNED($D$26+$D$27+1-$D$29,M32)</f>
+        <v>15536873272</v>
+      </c>
+      <c r="P32" s="2" cm="1">
+        <f t="array" ref="P32">UNSIGNED($D$26+$D$27+1-$D$29,N32)</f>
+        <v>625880919</v>
+      </c>
+      <c r="Q32" s="2" cm="1">
+        <f t="array" ref="Q32">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O32)</f>
+        <v>57144</v>
+      </c>
+      <c r="R32" s="2" cm="1">
+        <f t="array" ref="R32">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P32)</f>
+        <v>12119</v>
+      </c>
+      <c r="S32" s="2" cm="1">
+        <f t="array" ref="S32">SIGNED($D$28,Q32)</f>
+        <v>-8392</v>
+      </c>
+      <c r="T32" s="2" cm="1">
+        <f t="array" ref="T32">SIGNED($D$28,R32)</f>
+        <v>12119</v>
+      </c>
+    </row>
+    <row r="33" spans="4:20">
+      <c r="F33" s="1">
+        <v>5</v>
+      </c>
+      <c r="G33" s="9">
+        <v>108696</v>
+      </c>
+      <c r="H33" s="9">
+        <v>-31760</v>
+      </c>
+      <c r="I33" s="9">
+        <v>222482</v>
+      </c>
+      <c r="J33" s="9">
+        <v>-205476</v>
+      </c>
+      <c r="K33" s="2">
+        <f t="shared" si="1"/>
+        <v>17656985712</v>
+      </c>
+      <c r="L33" s="2">
+        <f t="shared" si="2"/>
+        <v>-29400447616</v>
+      </c>
+      <c r="M33" s="2" cm="1">
+        <f t="array" ref="M33">ROUND_INT_HF2EVN($D$29,K33)</f>
+        <v>1103561607</v>
+      </c>
+      <c r="N33" s="2" cm="1">
+        <f t="array" ref="N33">ROUND_INT_HF2EVN($D$29,L33)</f>
+        <v>-1837527976</v>
+      </c>
+      <c r="O33" s="2" cm="1">
+        <f t="array" ref="O33">UNSIGNED($D$26+$D$27+1-$D$29,M33)</f>
+        <v>1103561607</v>
+      </c>
+      <c r="P33" s="2" cm="1">
+        <f t="array" ref="P33">UNSIGNED($D$26+$D$27+1-$D$29,N33)</f>
+        <v>15342341208</v>
+      </c>
+      <c r="Q33" s="2" cm="1">
+        <f t="array" ref="Q33">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O33)</f>
+        <v>903</v>
+      </c>
+      <c r="R33" s="2" cm="1">
+        <f t="array" ref="R33">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P33)</f>
+        <v>35928</v>
+      </c>
+      <c r="S33" s="2" cm="1">
+        <f t="array" ref="S33">SIGNED($D$28,Q33)</f>
+        <v>903</v>
+      </c>
+      <c r="T33" s="2" cm="1">
+        <f t="array" ref="T33">SIGNED($D$28,R33)</f>
+        <v>-29608</v>
+      </c>
+    </row>
+    <row r="34" spans="4:20">
+      <c r="F34" s="1">
+        <v>6</v>
+      </c>
+      <c r="G34" s="9">
+        <v>-125839</v>
+      </c>
+      <c r="H34" s="9">
+        <v>66612</v>
+      </c>
+      <c r="I34" s="9">
+        <v>-225429</v>
+      </c>
+      <c r="J34" s="9">
+        <v>16826</v>
+      </c>
+      <c r="K34" s="2">
+        <f t="shared" si="1"/>
+        <v>27246946419</v>
+      </c>
+      <c r="L34" s="2">
+        <f t="shared" si="2"/>
+        <v>-17133643562</v>
+      </c>
+      <c r="M34" s="2" cm="1">
+        <f t="array" ref="M34">ROUND_INT_HF2EVN($D$29,K34)</f>
+        <v>1702934151</v>
+      </c>
+      <c r="N34" s="2" cm="1">
+        <f t="array" ref="N34">ROUND_INT_HF2EVN($D$29,L34)</f>
+        <v>-1070852723</v>
+      </c>
+      <c r="O34" s="2" cm="1">
+        <f t="array" ref="O34">UNSIGNED($D$26+$D$27+1-$D$29,M34)</f>
+        <v>1702934151</v>
+      </c>
+      <c r="P34" s="2" cm="1">
+        <f t="array" ref="P34">UNSIGNED($D$26+$D$27+1-$D$29,N34)</f>
+        <v>16109016461</v>
+      </c>
+      <c r="Q34" s="2" cm="1">
+        <f t="array" ref="Q34">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O34)</f>
+        <v>46727</v>
+      </c>
+      <c r="R34" s="2" cm="1">
+        <f t="array" ref="R34">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P34)</f>
+        <v>5517</v>
+      </c>
+      <c r="S34" s="2" cm="1">
+        <f t="array" ref="S34">SIGNED($D$28,Q34)</f>
+        <v>-18809</v>
+      </c>
+      <c r="T34" s="2" cm="1">
+        <f t="array" ref="T34">SIGNED($D$28,R34)</f>
+        <v>5517</v>
+      </c>
+    </row>
+    <row r="35" spans="4:20">
+      <c r="F35" s="1">
+        <v>7</v>
+      </c>
+      <c r="G35" s="9">
+        <v>30335</v>
+      </c>
+      <c r="H35" s="9">
+        <v>-34418</v>
+      </c>
+      <c r="I35" s="9">
+        <v>199780</v>
+      </c>
+      <c r="J35" s="9">
+        <v>-27879</v>
+      </c>
+      <c r="K35" s="2">
+        <f t="shared" si="1"/>
+        <v>5100786878</v>
+      </c>
+      <c r="L35" s="2">
+        <f t="shared" si="2"/>
+        <v>-7721737505</v>
+      </c>
+      <c r="M35" s="2" cm="1">
+        <f t="array" ref="M35">ROUND_INT_HF2EVN($D$29,K35)</f>
+        <v>318799180</v>
+      </c>
+      <c r="N35" s="2" cm="1">
+        <f t="array" ref="N35">ROUND_INT_HF2EVN($D$29,L35)</f>
+        <v>-482608594</v>
+      </c>
+      <c r="O35" s="2" cm="1">
+        <f t="array" ref="O35">UNSIGNED($D$26+$D$27+1-$D$29,M35)</f>
+        <v>318799180</v>
+      </c>
+      <c r="P35" s="2" cm="1">
+        <f t="array" ref="P35">UNSIGNED($D$26+$D$27+1-$D$29,N35)</f>
+        <v>16697260590</v>
+      </c>
+      <c r="Q35" s="2" cm="1">
+        <f t="array" ref="Q35">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O35)</f>
+        <v>32076</v>
+      </c>
+      <c r="R35" s="2" cm="1">
+        <f t="array" ref="R35">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P35)</f>
+        <v>64046</v>
+      </c>
+      <c r="S35" s="2" cm="1">
+        <f t="array" ref="S35">SIGNED($D$28,Q35)</f>
+        <v>32076</v>
+      </c>
+      <c r="T35" s="2" cm="1">
+        <f t="array" ref="T35">SIGNED($D$28,R35)</f>
+        <v>-1490</v>
+      </c>
+    </row>
+    <row r="36" spans="4:20">
+      <c r="F36" s="1">
+        <v>8</v>
+      </c>
+      <c r="G36" s="9">
+        <v>72389</v>
+      </c>
+      <c r="H36" s="9">
+        <v>81523</v>
+      </c>
+      <c r="I36" s="9">
+        <v>-47378</v>
+      </c>
+      <c r="J36" s="9">
+        <v>-51687</v>
+      </c>
+      <c r="K36" s="2">
+        <f t="shared" si="1"/>
+        <v>784033259</v>
+      </c>
+      <c r="L36" s="2">
+        <f t="shared" si="2"/>
+        <v>-7603966937</v>
+      </c>
+      <c r="M36" s="2" cm="1">
+        <f t="array" ref="M36">ROUND_INT_HF2EVN($D$29,K36)</f>
+        <v>49002079</v>
+      </c>
+      <c r="N36" s="2" cm="1">
+        <f t="array" ref="N36">ROUND_INT_HF2EVN($D$29,L36)</f>
+        <v>-475247934</v>
+      </c>
+      <c r="O36" s="2" cm="1">
+        <f t="array" ref="O36">UNSIGNED($D$26+$D$27+1-$D$29,M36)</f>
+        <v>49002079</v>
+      </c>
+      <c r="P36" s="2" cm="1">
+        <f t="array" ref="P36">UNSIGNED($D$26+$D$27+1-$D$29,N36)</f>
+        <v>16704621250</v>
+      </c>
+      <c r="Q36" s="2" cm="1">
+        <f t="array" ref="Q36">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O36)</f>
+        <v>46687</v>
+      </c>
+      <c r="R36" s="2" cm="1">
+        <f t="array" ref="R36">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P36)</f>
+        <v>19138</v>
+      </c>
+      <c r="S36" s="2" cm="1">
+        <f t="array" ref="S36">SIGNED($D$28,Q36)</f>
+        <v>-18849</v>
+      </c>
+      <c r="T36" s="2" cm="1">
+        <f t="array" ref="T36">SIGNED($D$28,R36)</f>
+        <v>19138</v>
+      </c>
+    </row>
+    <row r="37" spans="4:20">
+      <c r="E37" s="3"/>
+      <c r="F37" s="1">
+        <v>9</v>
+      </c>
+      <c r="G37" s="9">
+        <v>-87654</v>
+      </c>
+      <c r="H37" s="9">
+        <v>-5283</v>
+      </c>
+      <c r="I37" s="9">
+        <v>117726</v>
+      </c>
+      <c r="J37" s="9">
+        <v>-203134</v>
+      </c>
+      <c r="K37" s="2">
+        <f t="shared" si="1"/>
+        <v>-11392311726</v>
+      </c>
+      <c r="L37" s="2">
+        <f t="shared" si="2"/>
+        <v>17183561178</v>
+      </c>
+      <c r="M37" s="2" cm="1">
+        <f t="array" ref="M37">ROUND_INT_HF2EVN($D$29,K37)</f>
+        <v>-712019483</v>
+      </c>
+      <c r="N37" s="2" cm="1">
+        <f t="array" ref="N37">ROUND_INT_HF2EVN($D$29,L37)</f>
+        <v>1073972574</v>
+      </c>
+      <c r="O37" s="2" cm="1">
+        <f t="array" ref="O37">UNSIGNED($D$26+$D$27+1-$D$29,M37)</f>
+        <v>16467849701</v>
+      </c>
+      <c r="P37" s="2" cm="1">
+        <f t="array" ref="P37">UNSIGNED($D$26+$D$27+1-$D$29,N37)</f>
+        <v>1073972574</v>
+      </c>
+      <c r="Q37" s="2" cm="1">
+        <f t="array" ref="Q37">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O37)</f>
+        <v>29157</v>
+      </c>
+      <c r="R37" s="2" cm="1">
+        <f t="array" ref="R37">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P37)</f>
+        <v>34142</v>
+      </c>
+      <c r="S37" s="2" cm="1">
+        <f t="array" ref="S37">SIGNED($D$28,Q37)</f>
+        <v>29157</v>
+      </c>
+      <c r="T37" s="2" cm="1">
+        <f t="array" ref="T37">SIGNED($D$28,R37)</f>
+        <v>-31394</v>
+      </c>
+    </row>
+    <row r="38" spans="4:20">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="1">
+        <v>10</v>
+      </c>
+      <c r="G38" s="9">
+        <v>-118328</v>
+      </c>
+      <c r="H38" s="9">
+        <v>80912</v>
+      </c>
+      <c r="I38" s="9">
+        <v>-159965</v>
+      </c>
+      <c r="J38" s="9">
+        <v>-161301</v>
+      </c>
+      <c r="K38" s="2">
+        <f t="shared" si="1"/>
+        <v>31979525032</v>
+      </c>
+      <c r="L38" s="2">
+        <f t="shared" si="2"/>
+        <v>6143336648</v>
+      </c>
+      <c r="M38" s="2" cm="1">
+        <f t="array" ref="M38">ROUND_INT_HF2EVN($D$29,K38)</f>
+        <v>1998720314</v>
+      </c>
+      <c r="N38" s="2" cm="1">
+        <f t="array" ref="N38">ROUND_INT_HF2EVN($D$29,L38)</f>
+        <v>383958540</v>
+      </c>
+      <c r="O38" s="2" cm="1">
+        <f t="array" ref="O38">UNSIGNED($D$26+$D$27+1-$D$29,M38)</f>
+        <v>1998720314</v>
+      </c>
+      <c r="P38" s="2" cm="1">
+        <f t="array" ref="P38">UNSIGNED($D$26+$D$27+1-$D$29,N38)</f>
+        <v>383958540</v>
+      </c>
+      <c r="Q38" s="2" cm="1">
+        <f t="array" ref="Q38">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O38)</f>
+        <v>3386</v>
+      </c>
+      <c r="R38" s="2" cm="1">
+        <f t="array" ref="R38">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P38)</f>
+        <v>48652</v>
+      </c>
+      <c r="S38" s="2" cm="1">
+        <f t="array" ref="S38">SIGNED($D$28,Q38)</f>
+        <v>3386</v>
+      </c>
+      <c r="T38" s="2" cm="1">
+        <f t="array" ref="T38">SIGNED($D$28,R38)</f>
+        <v>-16884</v>
+      </c>
+    </row>
+    <row r="39" spans="4:20">
+      <c r="F39" s="1">
+        <v>11</v>
+      </c>
+      <c r="G39" s="9">
+        <v>34555</v>
+      </c>
+      <c r="H39" s="9">
+        <v>54757</v>
+      </c>
+      <c r="I39" s="9">
+        <v>-137129</v>
+      </c>
+      <c r="J39" s="9">
+        <v>26326</v>
+      </c>
+      <c r="K39" s="2">
+        <f t="shared" si="1"/>
+        <v>-6180025377</v>
+      </c>
+      <c r="L39" s="2">
+        <f t="shared" si="2"/>
+        <v>-6599077723</v>
+      </c>
+      <c r="M39" s="2" cm="1">
+        <f t="array" ref="M39">ROUND_INT_HF2EVN($D$29,K39)</f>
+        <v>-386251586</v>
+      </c>
+      <c r="N39" s="2" cm="1">
+        <f t="array" ref="N39">ROUND_INT_HF2EVN($D$29,L39)</f>
+        <v>-412442358</v>
+      </c>
+      <c r="O39" s="2" cm="1">
+        <f t="array" ref="O39">UNSIGNED($D$26+$D$27+1-$D$29,M39)</f>
+        <v>16793617598</v>
+      </c>
+      <c r="P39" s="2" cm="1">
+        <f t="array" ref="P39">UNSIGNED($D$26+$D$27+1-$D$29,N39)</f>
+        <v>16767426826</v>
+      </c>
+      <c r="Q39" s="2" cm="1">
+        <f t="array" ref="Q39">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O39)</f>
+        <v>17598</v>
+      </c>
+      <c r="R39" s="2" cm="1">
+        <f t="array" ref="R39">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P39)</f>
+        <v>41226</v>
+      </c>
+      <c r="S39" s="2" cm="1">
+        <f t="array" ref="S39">SIGNED($D$28,Q39)</f>
+        <v>17598</v>
+      </c>
+      <c r="T39" s="2" cm="1">
+        <f t="array" ref="T39">SIGNED($D$28,R39)</f>
+        <v>-24310</v>
+      </c>
+    </row>
+    <row r="40" spans="4:20">
+      <c r="F40" s="1">
+        <v>12</v>
+      </c>
+      <c r="G40" s="9">
+        <v>60667</v>
+      </c>
+      <c r="H40" s="9">
+        <v>-101056</v>
+      </c>
+      <c r="I40" s="9">
+        <v>33091</v>
+      </c>
+      <c r="J40" s="9">
+        <v>62490</v>
+      </c>
+      <c r="K40" s="2">
+        <f t="shared" si="1"/>
+        <v>8322521137</v>
+      </c>
+      <c r="L40" s="2">
+        <f t="shared" si="2"/>
+        <v>447036734</v>
+      </c>
+      <c r="M40" s="2" cm="1">
+        <f t="array" ref="M40">ROUND_INT_HF2EVN($D$29,K40)</f>
+        <v>520157571</v>
+      </c>
+      <c r="N40" s="2" cm="1">
+        <f t="array" ref="N40">ROUND_INT_HF2EVN($D$29,L40)</f>
+        <v>27939796</v>
+      </c>
+      <c r="O40" s="2" cm="1">
+        <f t="array" ref="O40">UNSIGNED($D$26+$D$27+1-$D$29,M40)</f>
+        <v>520157571</v>
+      </c>
+      <c r="P40" s="2" cm="1">
+        <f t="array" ref="P40">UNSIGNED($D$26+$D$27+1-$D$29,N40)</f>
+        <v>27939796</v>
+      </c>
+      <c r="Q40" s="2" cm="1">
+        <f t="array" ref="Q40">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O40)</f>
+        <v>63875</v>
+      </c>
+      <c r="R40" s="2" cm="1">
+        <f t="array" ref="R40">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P40)</f>
+        <v>21460</v>
+      </c>
+      <c r="S40" s="2" cm="1">
+        <f t="array" ref="S40">SIGNED($D$28,Q40)</f>
+        <v>-1661</v>
+      </c>
+      <c r="T40" s="2" cm="1">
+        <f t="array" ref="T40">SIGNED($D$28,R40)</f>
+        <v>21460</v>
+      </c>
+    </row>
+    <row r="41" spans="4:20">
+      <c r="F41" s="1">
+        <v>13</v>
+      </c>
+      <c r="G41" s="9">
+        <v>64139</v>
+      </c>
+      <c r="H41" s="9">
+        <v>-81752</v>
+      </c>
+      <c r="I41" s="9">
+        <v>-124157</v>
+      </c>
+      <c r="J41" s="9">
+        <v>-14465</v>
+      </c>
+      <c r="K41" s="2">
+        <f t="shared" si="1"/>
+        <v>-9145848503</v>
+      </c>
+      <c r="L41" s="2">
+        <f t="shared" si="2"/>
+        <v>9222312429</v>
+      </c>
+      <c r="M41" s="2" cm="1">
+        <f t="array" ref="M41">ROUND_INT_HF2EVN($D$29,K41)</f>
+        <v>-571615531</v>
+      </c>
+      <c r="N41" s="2" cm="1">
+        <f t="array" ref="N41">ROUND_INT_HF2EVN($D$29,L41)</f>
+        <v>576394527</v>
+      </c>
+      <c r="O41" s="2" cm="1">
+        <f t="array" ref="O41">UNSIGNED($D$26+$D$27+1-$D$29,M41)</f>
+        <v>16608253653</v>
+      </c>
+      <c r="P41" s="2" cm="1">
+        <f t="array" ref="P41">UNSIGNED($D$26+$D$27+1-$D$29,N41)</f>
+        <v>576394527</v>
+      </c>
+      <c r="Q41" s="2" cm="1">
+        <f t="array" ref="Q41">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O41)</f>
+        <v>54997</v>
+      </c>
+      <c r="R41" s="2" cm="1">
+        <f t="array" ref="R41">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P41)</f>
+        <v>5407</v>
+      </c>
+      <c r="S41" s="2" cm="1">
+        <f t="array" ref="S41">SIGNED($D$28,Q41)</f>
+        <v>-10539</v>
+      </c>
+      <c r="T41" s="2" cm="1">
+        <f t="array" ref="T41">SIGNED($D$28,R41)</f>
+        <v>5407</v>
+      </c>
+    </row>
+    <row r="42" spans="4:20">
+      <c r="F42" s="1">
+        <v>14</v>
+      </c>
+      <c r="G42" s="9">
+        <v>-102591</v>
+      </c>
+      <c r="H42" s="9">
+        <v>88015</v>
+      </c>
+      <c r="I42" s="9">
+        <v>150782</v>
+      </c>
+      <c r="J42" s="9">
+        <v>-174093</v>
+      </c>
+      <c r="K42" s="2">
+        <f t="shared" si="1"/>
+        <v>-146080767</v>
+      </c>
+      <c r="L42" s="2">
+        <f t="shared" si="2"/>
+        <v>31131452693</v>
+      </c>
+      <c r="M42" s="2" cm="1">
+        <f t="array" ref="M42">ROUND_INT_HF2EVN($D$29,K42)</f>
+        <v>-9130048</v>
+      </c>
+      <c r="N42" s="2" cm="1">
+        <f t="array" ref="N42">ROUND_INT_HF2EVN($D$29,L42)</f>
+        <v>1945715793</v>
+      </c>
+      <c r="O42" s="2" cm="1">
+        <f t="array" ref="O42">UNSIGNED($D$26+$D$27+1-$D$29,M42)</f>
+        <v>17170739136</v>
+      </c>
+      <c r="P42" s="2" cm="1">
+        <f t="array" ref="P42">UNSIGNED($D$26+$D$27+1-$D$29,N42)</f>
+        <v>1945715793</v>
+      </c>
+      <c r="Q42" s="2" cm="1">
+        <f t="array" ref="Q42">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O42)</f>
+        <v>44992</v>
+      </c>
+      <c r="R42" s="2" cm="1">
+        <f t="array" ref="R42">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P42)</f>
+        <v>17489</v>
+      </c>
+      <c r="S42" s="2" cm="1">
+        <f t="array" ref="S42">SIGNED($D$28,Q42)</f>
+        <v>-20544</v>
+      </c>
+      <c r="T42" s="2" cm="1">
+        <f t="array" ref="T42">SIGNED($D$28,R42)</f>
+        <v>17489</v>
+      </c>
+    </row>
+    <row r="43" spans="4:20">
+      <c r="F43" s="1">
+        <v>15</v>
+      </c>
+      <c r="G43" s="9">
+        <v>50998</v>
+      </c>
+      <c r="H43" s="9">
+        <v>-102247</v>
+      </c>
+      <c r="I43" s="9">
+        <v>148058</v>
+      </c>
+      <c r="J43" s="9">
+        <v>111038</v>
+      </c>
+      <c r="K43" s="2">
+        <f t="shared" si="1"/>
+        <v>18903964270</v>
+      </c>
+      <c r="L43" s="2">
+        <f t="shared" si="2"/>
+        <v>-9475770402</v>
+      </c>
+      <c r="M43" s="2" cm="1">
+        <f t="array" ref="M43">ROUND_INT_HF2EVN($D$29,K43)</f>
+        <v>1181497767</v>
+      </c>
+      <c r="N43" s="2" cm="1">
+        <f t="array" ref="N43">ROUND_INT_HF2EVN($D$29,L43)</f>
+        <v>-592235650</v>
+      </c>
+      <c r="O43" s="2" cm="1">
+        <f t="array" ref="O43">UNSIGNED($D$26+$D$27+1-$D$29,M43)</f>
+        <v>1181497767</v>
+      </c>
+      <c r="P43" s="2" cm="1">
+        <f t="array" ref="P43">UNSIGNED($D$26+$D$27+1-$D$29,N43)</f>
+        <v>16587633534</v>
+      </c>
+      <c r="Q43" s="2" cm="1">
+        <f t="array" ref="Q43">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,O43)</f>
+        <v>14759</v>
+      </c>
+      <c r="R43" s="2" cm="1">
+        <f t="array" ref="R43">BIT_SLICE($D$26+$D$27+1-$D$29,0,$D$28,P43)</f>
+        <v>13182</v>
+      </c>
+      <c r="S43" s="2" cm="1">
+        <f t="array" ref="S43">SIGNED($D$28,Q43)</f>
+        <v>14759</v>
+      </c>
+      <c r="T43" s="2" cm="1">
+        <f t="array" ref="T43">SIGNED($D$28,R43)</f>
+        <v>13182</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9">
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+    </row>
+    <row r="50" spans="4:9">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="7"/>
+    </row>
+    <row r="51" spans="4:9">
+      <c r="H51" s="3"/>
+    </row>
+    <row r="52" spans="4:9">
+      <c r="H52" s="3"/>
+    </row>
+    <row r="53" spans="4:9">
+      <c r="H53" s="3"/>
+    </row>
+    <row r="54" spans="4:9">
+      <c r="H54" s="3"/>
+    </row>
+    <row r="55" spans="4:9">
+      <c r="H55" s="3"/>
+    </row>
+    <row r="56" spans="4:9">
+      <c r="H56" s="3"/>
+    </row>
+    <row r="57" spans="4:9">
+      <c r="H57" s="3"/>
+    </row>
+    <row r="58" spans="4:9">
+      <c r="H58" s="3"/>
+    </row>
+    <row r="61" spans="4:9">
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="7"/>
+      <c r="I61" s="7"/>
+    </row>
+    <row r="62" spans="4:9">
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="D59:G59"/>
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="G47:G48"/>
-    <mergeCell ref="F2:J2"/>
-    <mergeCell ref="K2:N2"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="F35:F36"/>
+  <mergeCells count="21">
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="S26:S27"/>
+    <mergeCell ref="T26:T27"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="I61:I62"/>
+    <mergeCell ref="E61:H61"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
   </mergeCells>
-  <conditionalFormatting sqref="G49:G56">
+  <conditionalFormatting sqref="H51:H58 H26 H28:H43">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G20:G32">
+  <conditionalFormatting sqref="H22:H24">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>

</xml_diff>

<commit_message>
chore: fix Excel sheet name
</commit_message>
<xml_diff>
--- a/FPGA/synth/math/multiplier/sim/test_data.xlsx
+++ b/FPGA/synth/math/multiplier/sim/test_data.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="655" documentId="11_3F8216BDF2DCCE836B02CE998F0AE45F5E522874" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BFF8E6C-3083-4781-9AAF-2C8BECBDBEBC}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\motchy\Documents\GitHub\code-fractions\FPGA\synth\math\multiplier\sim\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C8B0E1-2088-4CBF-BBEE-AC2D72339EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="自作関数" sheetId="1" r:id="rId1"/>
+    <sheet name="test_data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="BIT_SLICE" comment="Extracts a bit slice with a given offset `offset` and bit width `BW_slice` from a given integer `x` with its bit width information `BW_orig`. The result is returned as an unsigned integer.">_xlfn.LAMBDA(_xlpm.BW_orig,_xlpm.offset,_xlpm.BW_slice,_xlpm.x,_xlfn.LET(_xlpm.us_x,UNSIGNED(_xlpm.BW_orig,_xlpm.x),_xlpm.y,_xlfn.BITRSHIFT(_xlpm.us_x,_xlpm.offset),_xlfn.BITAND(_xlpm.y,POWER(2,_xlpm.BW_slice)-1)))</definedName>
@@ -60,10 +65,19 @@
     </comment>
     <comment ref="G28" authorId="0" shapeId="0" xr:uid="{7913E922-01F6-4D70-9926-B43E91EB98AE}">
       <text>
-        <t>Motoki Kamimura:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="游ゴシック"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Motoki Kamimura:
 乱数で生成した後に再現性確保のために固定した。
 元の数式は下記：
 =LET(A,POWER(2,$D$26-1),RANDBETWEEN(-A,A-1))</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -71,7 +85,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -198,7 +212,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,7 +231,15 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="游ゴシック"/>
-      <charset val="1"/>
+      <family val="3"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -254,19 +276,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -625,59 +647,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="2" width="3.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="3.08203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.25" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" style="1"/>
     <col min="6" max="6" width="3.75" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="10" width="10" style="1" customWidth="1"/>
     <col min="11" max="11" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="15.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="15.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="9" style="1"/>
     <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:16">
+    <row r="2" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:16" ht="45" customHeight="1">
+    <row r="4" spans="2:16" ht="45" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C4" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="8" t="s">
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-      <c r="P4" s="7" t="s">
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:16" ht="39" customHeight="1">
+    <row r="5" spans="2:16" ht="39" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
@@ -711,9 +733,9 @@
       <c r="O5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="P5" s="7"/>
-    </row>
-    <row r="6" spans="2:16">
+      <c r="P5" s="8"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
@@ -759,7 +781,7 @@
         <v>3061</v>
       </c>
     </row>
-    <row r="7" spans="2:16">
+    <row r="7" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
@@ -805,7 +827,7 @@
         <v>-15858</v>
       </c>
     </row>
-    <row r="8" spans="2:16">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C8" s="1" t="s">
         <v>18</v>
       </c>
@@ -851,7 +873,7 @@
         <v>-12317</v>
       </c>
     </row>
-    <row r="9" spans="2:16">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C9" s="1" t="s">
         <v>19</v>
       </c>
@@ -897,7 +919,7 @@
         <v>5784</v>
       </c>
     </row>
-    <row r="10" spans="2:16">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="1" t="s">
         <v>20</v>
       </c>
@@ -943,7 +965,7 @@
         <v>-3037</v>
       </c>
     </row>
-    <row r="11" spans="2:16">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="C11" s="1" t="s">
         <v>21</v>
       </c>
@@ -989,7 +1011,7 @@
         <v>-24468</v>
       </c>
     </row>
-    <row r="12" spans="2:16">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F12" s="1">
         <v>6</v>
       </c>
@@ -1029,7 +1051,7 @@
         <v>-16226</v>
       </c>
     </row>
-    <row r="13" spans="2:16">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F13" s="1">
         <v>7</v>
       </c>
@@ -1069,7 +1091,7 @@
         <v>15380</v>
       </c>
     </row>
-    <row r="14" spans="2:16">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F14" s="1">
         <v>8</v>
       </c>
@@ -1109,7 +1131,7 @@
         <v>-21902</v>
       </c>
     </row>
-    <row r="15" spans="2:16">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F15" s="1">
         <v>9</v>
       </c>
@@ -1149,7 +1171,7 @@
         <v>-18568</v>
       </c>
     </row>
-    <row r="16" spans="2:16">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.55000000000000004">
       <c r="F16" s="1">
         <v>10</v>
       </c>
@@ -1189,7 +1211,7 @@
         <v>19186</v>
       </c>
     </row>
-    <row r="17" spans="2:20">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F17" s="1">
         <v>11</v>
       </c>
@@ -1229,7 +1251,7 @@
         <v>14442</v>
       </c>
     </row>
-    <row r="18" spans="2:20">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F18" s="1">
         <v>12</v>
       </c>
@@ -1269,7 +1291,7 @@
         <v>1983</v>
       </c>
     </row>
-    <row r="19" spans="2:20">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F19" s="1">
         <v>13</v>
       </c>
@@ -1309,7 +1331,7 @@
         <v>-17245</v>
       </c>
     </row>
-    <row r="20" spans="2:20">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F20" s="1">
         <v>14</v>
       </c>
@@ -1349,7 +1371,7 @@
         <v>-26312</v>
       </c>
     </row>
-    <row r="21" spans="2:20">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F21" s="1">
         <v>15</v>
       </c>
@@ -1389,99 +1411,99 @@
         <v>-14047</v>
       </c>
     </row>
-    <row r="22" spans="2:20">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="H22" s="3"/>
     </row>
-    <row r="23" spans="2:20">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" s="1" t="s">
         <v>22</v>
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="2:20">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="2:20">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C25" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="7" t="s">
+      <c r="G25" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H25" s="7"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="10" t="s">
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+      <c r="K25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="7" t="s">
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="T25" s="7"/>
-    </row>
-    <row r="26" spans="2:20">
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D26" s="1">
         <v>18</v>
       </c>
-      <c r="G26" s="7" t="s">
+      <c r="G26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I26" s="7" t="s">
+      <c r="I26" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="J26" s="7" t="s">
+      <c r="J26" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="K26" s="7" t="s">
+      <c r="K26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="L26" s="7"/>
-      <c r="M26" s="7" t="s">
+      <c r="L26" s="8"/>
+      <c r="M26" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="N26" s="7"/>
-      <c r="O26" s="7" t="s">
+      <c r="N26" s="8"/>
+      <c r="O26" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="P26" s="7"/>
-      <c r="Q26" s="7" t="s">
+      <c r="P26" s="8"/>
+      <c r="Q26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="R26" s="7"/>
-      <c r="S26" s="7" t="s">
+      <c r="R26" s="8"/>
+      <c r="S26" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="T26" s="7" t="s">
+      <c r="T26" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="2:20">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C27" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D27" s="1">
         <v>19</v>
       </c>
-      <c r="G27" s="7"/>
-      <c r="H27" s="7"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
       <c r="K27" s="3" t="s">
         <v>29</v>
       </c>
@@ -1506,10 +1528,10 @@
       <c r="R27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="S27" s="7"/>
-      <c r="T27" s="7"/>
-    </row>
-    <row r="28" spans="2:20">
+      <c r="S27" s="8"/>
+      <c r="T27" s="8"/>
+    </row>
+    <row r="28" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="1" t="s">
         <v>19</v>
       </c>
@@ -1519,16 +1541,16 @@
       <c r="F28" s="1">
         <v>0</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="7">
         <v>-28538</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="7">
         <v>-127202</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="7">
         <v>-184004</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="7">
         <v>13277</v>
       </c>
       <c r="K28" s="2">
@@ -1572,7 +1594,7 @@
         <v>3051</v>
       </c>
     </row>
-    <row r="29" spans="2:20">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C29" s="1" t="s">
         <v>20</v>
       </c>
@@ -1582,16 +1604,16 @@
       <c r="F29" s="1">
         <v>1</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="7">
         <v>106182</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="7">
         <v>-117151</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="7">
         <v>138179</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="7">
         <v>242635</v>
       </c>
       <c r="K29" s="2">
@@ -1635,7 +1657,7 @@
         <v>4094</v>
       </c>
     </row>
-    <row r="30" spans="2:20">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="C30" s="1" t="s">
         <v>21</v>
       </c>
@@ -1645,16 +1667,16 @@
       <c r="F30" s="1">
         <v>2</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <v>-7117</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="7">
         <v>80541</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="7">
         <v>175606</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="7">
         <v>147324</v>
       </c>
       <c r="K30" s="2">
@@ -1698,20 +1720,20 @@
         <v>22553</v>
       </c>
     </row>
-    <row r="31" spans="2:20">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F31" s="1">
         <v>3</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="7">
         <v>-119900</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="7">
         <v>-18819</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="7">
         <v>-16301</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="7">
         <v>107207</v>
       </c>
       <c r="K31" s="2">
@@ -1755,20 +1777,20 @@
         <v>-5648</v>
       </c>
     </row>
-    <row r="32" spans="2:20">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F32" s="1">
         <v>4</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="7">
         <v>107635</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="7">
         <v>-54437</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="7">
         <v>-231955</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="7">
         <v>-24275</v>
       </c>
       <c r="K32" s="2">
@@ -1812,20 +1834,20 @@
         <v>12119</v>
       </c>
     </row>
-    <row r="33" spans="4:20">
+    <row r="33" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F33" s="1">
         <v>5</v>
       </c>
-      <c r="G33" s="9">
+      <c r="G33" s="7">
         <v>108696</v>
       </c>
-      <c r="H33" s="9">
+      <c r="H33" s="7">
         <v>-31760</v>
       </c>
-      <c r="I33" s="9">
+      <c r="I33" s="7">
         <v>222482</v>
       </c>
-      <c r="J33" s="9">
+      <c r="J33" s="7">
         <v>-205476</v>
       </c>
       <c r="K33" s="2">
@@ -1869,20 +1891,20 @@
         <v>-29608</v>
       </c>
     </row>
-    <row r="34" spans="4:20">
+    <row r="34" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F34" s="1">
         <v>6</v>
       </c>
-      <c r="G34" s="9">
+      <c r="G34" s="7">
         <v>-125839</v>
       </c>
-      <c r="H34" s="9">
+      <c r="H34" s="7">
         <v>66612</v>
       </c>
-      <c r="I34" s="9">
+      <c r="I34" s="7">
         <v>-225429</v>
       </c>
-      <c r="J34" s="9">
+      <c r="J34" s="7">
         <v>16826</v>
       </c>
       <c r="K34" s="2">
@@ -1926,20 +1948,20 @@
         <v>5517</v>
       </c>
     </row>
-    <row r="35" spans="4:20">
+    <row r="35" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F35" s="1">
         <v>7</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="7">
         <v>30335</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="7">
         <v>-34418</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="7">
         <v>199780</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="7">
         <v>-27879</v>
       </c>
       <c r="K35" s="2">
@@ -1983,20 +2005,20 @@
         <v>-1490</v>
       </c>
     </row>
-    <row r="36" spans="4:20">
+    <row r="36" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F36" s="1">
         <v>8</v>
       </c>
-      <c r="G36" s="9">
+      <c r="G36" s="7">
         <v>72389</v>
       </c>
-      <c r="H36" s="9">
+      <c r="H36" s="7">
         <v>81523</v>
       </c>
-      <c r="I36" s="9">
+      <c r="I36" s="7">
         <v>-47378</v>
       </c>
-      <c r="J36" s="9">
+      <c r="J36" s="7">
         <v>-51687</v>
       </c>
       <c r="K36" s="2">
@@ -2040,21 +2062,21 @@
         <v>19138</v>
       </c>
     </row>
-    <row r="37" spans="4:20">
+    <row r="37" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="E37" s="3"/>
       <c r="F37" s="1">
         <v>9</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="7">
         <v>-87654</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="7">
         <v>-5283</v>
       </c>
-      <c r="I37" s="9">
+      <c r="I37" s="7">
         <v>117726</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37" s="7">
         <v>-203134</v>
       </c>
       <c r="K37" s="2">
@@ -2098,22 +2120,22 @@
         <v>-31394</v>
       </c>
     </row>
-    <row r="38" spans="4:20">
+    <row r="38" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
       <c r="F38" s="1">
         <v>10</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="7">
         <v>-118328</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="7">
         <v>80912</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="7">
         <v>-159965</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="7">
         <v>-161301</v>
       </c>
       <c r="K38" s="2">
@@ -2157,20 +2179,20 @@
         <v>-16884</v>
       </c>
     </row>
-    <row r="39" spans="4:20">
+    <row r="39" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F39" s="1">
         <v>11</v>
       </c>
-      <c r="G39" s="9">
+      <c r="G39" s="7">
         <v>34555</v>
       </c>
-      <c r="H39" s="9">
+      <c r="H39" s="7">
         <v>54757</v>
       </c>
-      <c r="I39" s="9">
+      <c r="I39" s="7">
         <v>-137129</v>
       </c>
-      <c r="J39" s="9">
+      <c r="J39" s="7">
         <v>26326</v>
       </c>
       <c r="K39" s="2">
@@ -2214,20 +2236,20 @@
         <v>-24310</v>
       </c>
     </row>
-    <row r="40" spans="4:20">
+    <row r="40" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F40" s="1">
         <v>12</v>
       </c>
-      <c r="G40" s="9">
+      <c r="G40" s="7">
         <v>60667</v>
       </c>
-      <c r="H40" s="9">
+      <c r="H40" s="7">
         <v>-101056</v>
       </c>
-      <c r="I40" s="9">
+      <c r="I40" s="7">
         <v>33091</v>
       </c>
-      <c r="J40" s="9">
+      <c r="J40" s="7">
         <v>62490</v>
       </c>
       <c r="K40" s="2">
@@ -2271,20 +2293,20 @@
         <v>21460</v>
       </c>
     </row>
-    <row r="41" spans="4:20">
+    <row r="41" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F41" s="1">
         <v>13</v>
       </c>
-      <c r="G41" s="9">
+      <c r="G41" s="7">
         <v>64139</v>
       </c>
-      <c r="H41" s="9">
+      <c r="H41" s="7">
         <v>-81752</v>
       </c>
-      <c r="I41" s="9">
+      <c r="I41" s="7">
         <v>-124157</v>
       </c>
-      <c r="J41" s="9">
+      <c r="J41" s="7">
         <v>-14465</v>
       </c>
       <c r="K41" s="2">
@@ -2328,20 +2350,20 @@
         <v>5407</v>
       </c>
     </row>
-    <row r="42" spans="4:20">
+    <row r="42" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F42" s="1">
         <v>14</v>
       </c>
-      <c r="G42" s="9">
+      <c r="G42" s="7">
         <v>-102591</v>
       </c>
-      <c r="H42" s="9">
+      <c r="H42" s="7">
         <v>88015</v>
       </c>
-      <c r="I42" s="9">
+      <c r="I42" s="7">
         <v>150782</v>
       </c>
-      <c r="J42" s="9">
+      <c r="J42" s="7">
         <v>-174093</v>
       </c>
       <c r="K42" s="2">
@@ -2385,20 +2407,20 @@
         <v>17489</v>
       </c>
     </row>
-    <row r="43" spans="4:20">
+    <row r="43" spans="4:20" x14ac:dyDescent="0.55000000000000004">
       <c r="F43" s="1">
         <v>15</v>
       </c>
-      <c r="G43" s="9">
+      <c r="G43" s="7">
         <v>50998</v>
       </c>
-      <c r="H43" s="9">
+      <c r="H43" s="7">
         <v>-102247</v>
       </c>
-      <c r="I43" s="9">
+      <c r="I43" s="7">
         <v>148058</v>
       </c>
-      <c r="J43" s="9">
+      <c r="J43" s="7">
         <v>111038</v>
       </c>
       <c r="K43" s="2">
@@ -2442,60 +2464,69 @@
         <v>13182</v>
       </c>
     </row>
-    <row r="49" spans="4:9">
-      <c r="E49" s="7"/>
-      <c r="F49" s="7"/>
-      <c r="G49" s="7"/>
-      <c r="H49" s="7"/>
-    </row>
-    <row r="50" spans="4:9">
+    <row r="49" spans="4:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="E49" s="8"/>
+      <c r="F49" s="8"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
-      <c r="G50" s="7"/>
-      <c r="H50" s="7"/>
-    </row>
-    <row r="51" spans="4:9">
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H51" s="3"/>
     </row>
-    <row r="52" spans="4:9">
+    <row r="52" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H52" s="3"/>
     </row>
-    <row r="53" spans="4:9">
+    <row r="53" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H53" s="3"/>
     </row>
-    <row r="54" spans="4:9">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H54" s="3"/>
     </row>
-    <row r="55" spans="4:9">
+    <row r="55" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H55" s="3"/>
     </row>
-    <row r="56" spans="4:9">
+    <row r="56" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H56" s="3"/>
     </row>
-    <row r="57" spans="4:9">
+    <row r="57" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H57" s="3"/>
     </row>
-    <row r="58" spans="4:9">
+    <row r="58" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="H58" s="3"/>
     </row>
-    <row r="61" spans="4:9">
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-      <c r="I61" s="7"/>
-    </row>
-    <row r="62" spans="4:9">
+    <row r="61" spans="4:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="E61" s="8"/>
+      <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.55000000000000004">
       <c r="D62" s="3"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="7"/>
+      <c r="I62" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="I61:I62"/>
+    <mergeCell ref="E61:H61"/>
+    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="H49:H50"/>
+    <mergeCell ref="G4:K4"/>
+    <mergeCell ref="L4:O4"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="G25:J25"/>
+    <mergeCell ref="E49:F49"/>
     <mergeCell ref="S25:T25"/>
     <mergeCell ref="G26:G27"/>
     <mergeCell ref="H26:H27"/>
@@ -2508,23 +2539,15 @@
     <mergeCell ref="O26:P26"/>
     <mergeCell ref="Q26:R26"/>
     <mergeCell ref="K25:R25"/>
-    <mergeCell ref="G4:K4"/>
-    <mergeCell ref="L4:O4"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="G25:J25"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="I61:I62"/>
-    <mergeCell ref="E61:H61"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="H49:H50"/>
   </mergeCells>
-  <conditionalFormatting sqref="H51:H58 H26 H28:H43">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <phoneticPr fontId="3"/>
+  <conditionalFormatting sqref="H22:H24">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H22:H24">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="H26 H28:H43 H51:H58">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"NG"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
chore: update docs in test pattern gen
</commit_message>
<xml_diff>
--- a/FPGA/synth/math/multiplier/sim/test_data.xlsx
+++ b/FPGA/synth/math/multiplier/sim/test_data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28110"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="751" documentId="11_3F8216BDF2DCCE836B02CE998F0AE45F5E522874" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{825E6ABB-30E5-4905-A24A-EC51A6ABBA25}"/>
+  <xr:revisionPtr revIDLastSave="752" documentId="11_3F8216BDF2DCCE836B02CE998F0AE45F5E522874" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4267321F-4C86-407E-8D9D-14A3B4EB080C}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,10 +45,19 @@
   <commentList>
     <comment ref="G6" authorId="0" shapeId="0" xr:uid="{2E60492E-1DA8-4D5E-A2BE-9B5D0F493EA6}">
       <text>
-        <t>Motoki Kamimura:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="游ゴシック"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Motoki Kamimura:
 乱数で生成した後に再現性確保のために固定した。
 元の数式は下記：
 =LET(A,POWER(2,$D$26-1),RANDBETWEEN(-A,A-1))</t>
+        </r>
       </text>
     </comment>
     <comment ref="G25" authorId="0" shapeId="0" xr:uid="{ADDE4464-8DFC-45ED-AFE4-38EAD8AD5580}">
@@ -68,10 +77,19 @@
     </comment>
     <comment ref="G27" authorId="0" shapeId="0" xr:uid="{60E8420D-E157-4229-BF63-BF8E0C4B1B3E}">
       <text>
-        <t>Motoki Kamimura:
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="游ゴシック"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Motoki Kamimura:
 乱数で生成した後に再現性確保のために固定した。
 元の数式は下記：
 =LET(A,POWER(2,$D$26-1),RANDBETWEEN(-A,A-1))</t>
+        </r>
       </text>
     </comment>
     <comment ref="G49" authorId="0" shapeId="0" xr:uid="{7913E922-01F6-4D70-9926-B43E91EB98AE}">
@@ -120,7 +138,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="40">
   <si>
-    <t>test_bench_fxd_pt_mul_v2_0_0</t>
+    <t>test_bench_fxd_pt_mul_v2_1_0</t>
   </si>
   <si>
     <t>parameter</t>
@@ -299,23 +317,23 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,7 +693,7 @@
   <dimension ref="B2:T83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
@@ -704,10 +722,10 @@
       </c>
     </row>
     <row r="4" spans="2:13">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -731,22 +749,22 @@
       <c r="D5" s="1">
         <v>16</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="G5" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="M5" s="8"/>
@@ -1277,10 +1295,10 @@
       </c>
     </row>
     <row r="25" spans="2:16" ht="45" customHeight="1">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G25" s="8" t="s">
@@ -1290,12 +1308,12 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8"/>
-      <c r="L25" s="10" t="s">
+      <c r="L25" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
       <c r="P25" s="8" t="s">
         <v>5</v>
       </c>
@@ -1307,31 +1325,31 @@
       <c r="D26" s="1">
         <v>18</v>
       </c>
-      <c r="G26" s="5" t="s">
+      <c r="G26" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H26" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="I26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="K26" s="5" t="s">
+      <c r="K26" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="L26" s="6" t="s">
+      <c r="L26" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="M26" s="5" t="s">
+      <c r="M26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="N26" s="5" t="s">
+      <c r="N26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="O26" s="5" t="s">
+      <c r="O26" s="6" t="s">
         <v>12</v>
       </c>
       <c r="P26" s="8"/>
@@ -2013,22 +2031,22 @@
       </c>
     </row>
     <row r="43" spans="2:20">
-      <c r="H43" s="5"/>
+      <c r="H43" s="6"/>
     </row>
     <row r="44" spans="2:20">
       <c r="B44" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H44" s="5"/>
+      <c r="H44" s="6"/>
     </row>
     <row r="45" spans="2:20">
-      <c r="H45" s="5"/>
+      <c r="H45" s="6"/>
     </row>
     <row r="46" spans="2:20">
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="6" t="s">
         <v>2</v>
       </c>
       <c r="G46" s="8" t="s">
@@ -2037,16 +2055,16 @@
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
       <c r="J46" s="8"/>
-      <c r="K46" s="9" t="s">
+      <c r="K46" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
+      <c r="L46" s="10"/>
+      <c r="M46" s="10"/>
+      <c r="N46" s="10"/>
+      <c r="O46" s="10"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="10"/>
+      <c r="R46" s="10"/>
       <c r="S46" s="8" t="s">
         <v>5</v>
       </c>
@@ -2105,28 +2123,28 @@
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="5" t="s">
+      <c r="K48" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="L48" s="5" t="s">
+      <c r="L48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="M48" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N48" s="5" t="s">
+      <c r="N48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O48" s="5" t="s">
+      <c r="O48" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="P48" s="5" t="s">
+      <c r="P48" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="Q48" s="5" t="s">
+      <c r="Q48" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="R48" s="5" t="s">
+      <c r="R48" s="6" t="s">
         <v>38</v>
       </c>
       <c r="S48" s="8"/>
@@ -2142,16 +2160,16 @@
       <c r="F49" s="1">
         <v>0</v>
       </c>
-      <c r="G49" s="7">
+      <c r="G49" s="5">
         <v>-28538</v>
       </c>
-      <c r="H49" s="7">
+      <c r="H49" s="5">
         <v>-127202</v>
       </c>
-      <c r="I49" s="7">
+      <c r="I49" s="5">
         <v>-184004</v>
       </c>
-      <c r="J49" s="7">
+      <c r="J49" s="5">
         <v>13277</v>
       </c>
       <c r="K49" s="2">
@@ -2205,16 +2223,16 @@
       <c r="F50" s="1">
         <v>1</v>
       </c>
-      <c r="G50" s="7">
+      <c r="G50" s="5">
         <v>106182</v>
       </c>
-      <c r="H50" s="7">
+      <c r="H50" s="5">
         <v>-117151</v>
       </c>
-      <c r="I50" s="7">
+      <c r="I50" s="5">
         <v>138179</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="5">
         <v>242635</v>
       </c>
       <c r="K50" s="2">
@@ -2268,16 +2286,16 @@
       <c r="F51" s="1">
         <v>2</v>
       </c>
-      <c r="G51" s="7">
+      <c r="G51" s="5">
         <v>-7117</v>
       </c>
-      <c r="H51" s="7">
+      <c r="H51" s="5">
         <v>80541</v>
       </c>
-      <c r="I51" s="7">
+      <c r="I51" s="5">
         <v>175606</v>
       </c>
-      <c r="J51" s="7">
+      <c r="J51" s="5">
         <v>147324</v>
       </c>
       <c r="K51" s="2">
@@ -2325,16 +2343,16 @@
       <c r="F52" s="1">
         <v>3</v>
       </c>
-      <c r="G52" s="7">
+      <c r="G52" s="5">
         <v>-119900</v>
       </c>
-      <c r="H52" s="7">
+      <c r="H52" s="5">
         <v>-18819</v>
       </c>
-      <c r="I52" s="7">
+      <c r="I52" s="5">
         <v>-16301</v>
       </c>
-      <c r="J52" s="7">
+      <c r="J52" s="5">
         <v>107207</v>
       </c>
       <c r="K52" s="2">
@@ -2382,16 +2400,16 @@
       <c r="F53" s="1">
         <v>4</v>
       </c>
-      <c r="G53" s="7">
+      <c r="G53" s="5">
         <v>107635</v>
       </c>
-      <c r="H53" s="7">
+      <c r="H53" s="5">
         <v>-54437</v>
       </c>
-      <c r="I53" s="7">
+      <c r="I53" s="5">
         <v>-231955</v>
       </c>
-      <c r="J53" s="7">
+      <c r="J53" s="5">
         <v>-24275</v>
       </c>
       <c r="K53" s="2">
@@ -2439,16 +2457,16 @@
       <c r="F54" s="1">
         <v>5</v>
       </c>
-      <c r="G54" s="7">
+      <c r="G54" s="5">
         <v>108696</v>
       </c>
-      <c r="H54" s="7">
+      <c r="H54" s="5">
         <v>-31760</v>
       </c>
-      <c r="I54" s="7">
+      <c r="I54" s="5">
         <v>222482</v>
       </c>
-      <c r="J54" s="7">
+      <c r="J54" s="5">
         <v>-205476</v>
       </c>
       <c r="K54" s="2">
@@ -2496,16 +2514,16 @@
       <c r="F55" s="1">
         <v>6</v>
       </c>
-      <c r="G55" s="7">
+      <c r="G55" s="5">
         <v>-125839</v>
       </c>
-      <c r="H55" s="7">
+      <c r="H55" s="5">
         <v>66612</v>
       </c>
-      <c r="I55" s="7">
+      <c r="I55" s="5">
         <v>-225429</v>
       </c>
-      <c r="J55" s="7">
+      <c r="J55" s="5">
         <v>16826</v>
       </c>
       <c r="K55" s="2">
@@ -2553,16 +2571,16 @@
       <c r="F56" s="1">
         <v>7</v>
       </c>
-      <c r="G56" s="7">
+      <c r="G56" s="5">
         <v>30335</v>
       </c>
-      <c r="H56" s="7">
+      <c r="H56" s="5">
         <v>-34418</v>
       </c>
-      <c r="I56" s="7">
+      <c r="I56" s="5">
         <v>199780</v>
       </c>
-      <c r="J56" s="7">
+      <c r="J56" s="5">
         <v>-27879</v>
       </c>
       <c r="K56" s="2">
@@ -2610,16 +2628,16 @@
       <c r="F57" s="1">
         <v>8</v>
       </c>
-      <c r="G57" s="7">
+      <c r="G57" s="5">
         <v>72389</v>
       </c>
-      <c r="H57" s="7">
+      <c r="H57" s="5">
         <v>81523</v>
       </c>
-      <c r="I57" s="7">
+      <c r="I57" s="5">
         <v>-47378</v>
       </c>
-      <c r="J57" s="7">
+      <c r="J57" s="5">
         <v>-51687</v>
       </c>
       <c r="K57" s="2">
@@ -2664,20 +2682,20 @@
       </c>
     </row>
     <row r="58" spans="3:20">
-      <c r="E58" s="5"/>
+      <c r="E58" s="6"/>
       <c r="F58" s="1">
         <v>9</v>
       </c>
-      <c r="G58" s="7">
+      <c r="G58" s="5">
         <v>-87654</v>
       </c>
-      <c r="H58" s="7">
+      <c r="H58" s="5">
         <v>-5283</v>
       </c>
-      <c r="I58" s="7">
+      <c r="I58" s="5">
         <v>117726</v>
       </c>
-      <c r="J58" s="7">
+      <c r="J58" s="5">
         <v>-203134</v>
       </c>
       <c r="K58" s="2">
@@ -2722,21 +2740,21 @@
       </c>
     </row>
     <row r="59" spans="3:20">
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
       <c r="F59" s="1">
         <v>10</v>
       </c>
-      <c r="G59" s="7">
+      <c r="G59" s="5">
         <v>-118328</v>
       </c>
-      <c r="H59" s="7">
+      <c r="H59" s="5">
         <v>80912</v>
       </c>
-      <c r="I59" s="7">
+      <c r="I59" s="5">
         <v>-159965</v>
       </c>
-      <c r="J59" s="7">
+      <c r="J59" s="5">
         <v>-161301</v>
       </c>
       <c r="K59" s="2">
@@ -2784,16 +2802,16 @@
       <c r="F60" s="1">
         <v>11</v>
       </c>
-      <c r="G60" s="7">
+      <c r="G60" s="5">
         <v>34555</v>
       </c>
-      <c r="H60" s="7">
+      <c r="H60" s="5">
         <v>54757</v>
       </c>
-      <c r="I60" s="7">
+      <c r="I60" s="5">
         <v>-137129</v>
       </c>
-      <c r="J60" s="7">
+      <c r="J60" s="5">
         <v>26326</v>
       </c>
       <c r="K60" s="2">
@@ -2841,16 +2859,16 @@
       <c r="F61" s="1">
         <v>12</v>
       </c>
-      <c r="G61" s="7">
+      <c r="G61" s="5">
         <v>60667</v>
       </c>
-      <c r="H61" s="7">
+      <c r="H61" s="5">
         <v>-101056</v>
       </c>
-      <c r="I61" s="7">
+      <c r="I61" s="5">
         <v>33091</v>
       </c>
-      <c r="J61" s="7">
+      <c r="J61" s="5">
         <v>62490</v>
       </c>
       <c r="K61" s="2">
@@ -2898,16 +2916,16 @@
       <c r="F62" s="1">
         <v>13</v>
       </c>
-      <c r="G62" s="7">
+      <c r="G62" s="5">
         <v>64139</v>
       </c>
-      <c r="H62" s="7">
+      <c r="H62" s="5">
         <v>-81752</v>
       </c>
-      <c r="I62" s="7">
+      <c r="I62" s="5">
         <v>-124157</v>
       </c>
-      <c r="J62" s="7">
+      <c r="J62" s="5">
         <v>-14465</v>
       </c>
       <c r="K62" s="2">
@@ -2955,16 +2973,16 @@
       <c r="F63" s="1">
         <v>14</v>
       </c>
-      <c r="G63" s="7">
+      <c r="G63" s="5">
         <v>-102591</v>
       </c>
-      <c r="H63" s="7">
+      <c r="H63" s="5">
         <v>88015</v>
       </c>
-      <c r="I63" s="7">
+      <c r="I63" s="5">
         <v>150782</v>
       </c>
-      <c r="J63" s="7">
+      <c r="J63" s="5">
         <v>-174093</v>
       </c>
       <c r="K63" s="2">
@@ -3012,16 +3030,16 @@
       <c r="F64" s="1">
         <v>15</v>
       </c>
-      <c r="G64" s="7">
+      <c r="G64" s="5">
         <v>50998</v>
       </c>
-      <c r="H64" s="7">
+      <c r="H64" s="5">
         <v>-102247</v>
       </c>
-      <c r="I64" s="7">
+      <c r="I64" s="5">
         <v>148058</v>
       </c>
-      <c r="J64" s="7">
+      <c r="J64" s="5">
         <v>111038</v>
       </c>
       <c r="K64" s="2">
@@ -3072,35 +3090,35 @@
       <c r="H70" s="8"/>
     </row>
     <row r="71" spans="4:8">
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
     </row>
     <row r="72" spans="4:8">
-      <c r="H72" s="5"/>
+      <c r="H72" s="6"/>
     </row>
     <row r="73" spans="4:8">
-      <c r="H73" s="5"/>
+      <c r="H73" s="6"/>
     </row>
     <row r="74" spans="4:8">
-      <c r="H74" s="5"/>
+      <c r="H74" s="6"/>
     </row>
     <row r="75" spans="4:8">
-      <c r="H75" s="5"/>
+      <c r="H75" s="6"/>
     </row>
     <row r="76" spans="4:8">
-      <c r="H76" s="5"/>
+      <c r="H76" s="6"/>
     </row>
     <row r="77" spans="4:8">
-      <c r="H77" s="5"/>
+      <c r="H77" s="6"/>
     </row>
     <row r="78" spans="4:8">
-      <c r="H78" s="5"/>
+      <c r="H78" s="6"/>
     </row>
     <row r="79" spans="4:8">
-      <c r="H79" s="5"/>
+      <c r="H79" s="6"/>
     </row>
     <row r="82" spans="4:9">
       <c r="E82" s="8"/>
@@ -3110,24 +3128,15 @@
       <c r="I82" s="8"/>
     </row>
     <row r="83" spans="4:9">
-      <c r="D83" s="5"/>
-      <c r="E83" s="5"/>
-      <c r="F83" s="5"/>
-      <c r="G83" s="5"/>
-      <c r="H83" s="5"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
       <c r="I83" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="I82:I83"/>
-    <mergeCell ref="E82:H82"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="H70:H71"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="I4:L4"/>
-    <mergeCell ref="G25:K25"/>
-    <mergeCell ref="L25:O25"/>
     <mergeCell ref="P25:P26"/>
     <mergeCell ref="G46:J46"/>
     <mergeCell ref="E70:F70"/>
@@ -3143,6 +3152,15 @@
     <mergeCell ref="O47:P47"/>
     <mergeCell ref="Q47:R47"/>
     <mergeCell ref="K46:R46"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="I82:I83"/>
+    <mergeCell ref="E82:H82"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="I4:L4"/>
+    <mergeCell ref="G25:K25"/>
+    <mergeCell ref="L25:O25"/>
   </mergeCells>
   <conditionalFormatting sqref="H72:H79 H47 H49:H64">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>